<commit_message>
Measured benchmarks for set partitioning.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F0EBEF-0A94-40DA-83F6-F325D9D7434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C0A191-67CB-4031-9C93-CC324F3B6BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Integer Partitioning" sheetId="1" r:id="rId1"/>
+    <sheet name="Set Partitioning" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="259">
   <si>
     <t>TREE (n/k)</t>
   </si>
@@ -258,6 +259,561 @@
   </si>
   <si>
     <t>122736512us</t>
+  </si>
+  <si>
+    <t>185905658us</t>
+  </si>
+  <si>
+    <t>277380702us</t>
+  </si>
+  <si>
+    <t>404457022us</t>
+  </si>
+  <si>
+    <t>2667us</t>
+  </si>
+  <si>
+    <t>161661us</t>
+  </si>
+  <si>
+    <t>1830271us</t>
+  </si>
+  <si>
+    <t>8451274us</t>
+  </si>
+  <si>
+    <t>31533810us</t>
+  </si>
+  <si>
+    <t>92634376us</t>
+  </si>
+  <si>
+    <t>224277937us</t>
+  </si>
+  <si>
+    <t>6774us</t>
+  </si>
+  <si>
+    <t>631320us</t>
+  </si>
+  <si>
+    <t>9172419us</t>
+  </si>
+  <si>
+    <t>63839548us</t>
+  </si>
+  <si>
+    <t>285070698us</t>
+  </si>
+  <si>
+    <t>12729us</t>
+  </si>
+  <si>
+    <t>2042612us</t>
+  </si>
+  <si>
+    <t>40767836us</t>
+  </si>
+  <si>
+    <t>375919353us</t>
+  </si>
+  <si>
+    <t>22714us</t>
+  </si>
+  <si>
+    <t>5785519us</t>
+  </si>
+  <si>
+    <t>159831163us</t>
+  </si>
+  <si>
+    <t>CONJ (n/k)</t>
+  </si>
+  <si>
+    <t>691us</t>
+  </si>
+  <si>
+    <t>2312us</t>
+  </si>
+  <si>
+    <t>5779us</t>
+  </si>
+  <si>
+    <t>11358us</t>
+  </si>
+  <si>
+    <t>22025us</t>
+  </si>
+  <si>
+    <t>30134us</t>
+  </si>
+  <si>
+    <t>47378us</t>
+  </si>
+  <si>
+    <t>61126us</t>
+  </si>
+  <si>
+    <t>84652us</t>
+  </si>
+  <si>
+    <t>109579us</t>
+  </si>
+  <si>
+    <t>167127us</t>
+  </si>
+  <si>
+    <t>205102us</t>
+  </si>
+  <si>
+    <t>255136us</t>
+  </si>
+  <si>
+    <t>310589us</t>
+  </si>
+  <si>
+    <t>740998us</t>
+  </si>
+  <si>
+    <t>2623519us</t>
+  </si>
+  <si>
+    <t>6387292us</t>
+  </si>
+  <si>
+    <t>13199726us</t>
+  </si>
+  <si>
+    <t>107600473us</t>
+  </si>
+  <si>
+    <t>547us</t>
+  </si>
+  <si>
+    <t>9438us</t>
+  </si>
+  <si>
+    <t>76432us</t>
+  </si>
+  <si>
+    <t>147282us</t>
+  </si>
+  <si>
+    <t>341708us</t>
+  </si>
+  <si>
+    <t>699692us</t>
+  </si>
+  <si>
+    <t>1224674us</t>
+  </si>
+  <si>
+    <t>2078619us</t>
+  </si>
+  <si>
+    <t>3432289us</t>
+  </si>
+  <si>
+    <t>5785735us</t>
+  </si>
+  <si>
+    <t>7586864us</t>
+  </si>
+  <si>
+    <t>10750984us</t>
+  </si>
+  <si>
+    <t>14872826us</t>
+  </si>
+  <si>
+    <t>20250311us</t>
+  </si>
+  <si>
+    <t>26848032us</t>
+  </si>
+  <si>
+    <t>88141193us</t>
+  </si>
+  <si>
+    <t>515176526us</t>
+  </si>
+  <si>
+    <t>2323us</t>
+  </si>
+  <si>
+    <t>75517us</t>
+  </si>
+  <si>
+    <t>560899us</t>
+  </si>
+  <si>
+    <t>2333673us</t>
+  </si>
+  <si>
+    <t>6524722us</t>
+  </si>
+  <si>
+    <t>17858608us</t>
+  </si>
+  <si>
+    <t>35094725us</t>
+  </si>
+  <si>
+    <t>69031881us</t>
+  </si>
+  <si>
+    <t>124747219us</t>
+  </si>
+  <si>
+    <t>7154us</t>
+  </si>
+  <si>
+    <t>452701us</t>
+  </si>
+  <si>
+    <t>4541782us</t>
+  </si>
+  <si>
+    <t>24912885us</t>
+  </si>
+  <si>
+    <t>95316304us</t>
+  </si>
+  <si>
+    <t>279769536us</t>
+  </si>
+  <si>
+    <t>24931us</t>
+  </si>
+  <si>
+    <t>2076576us</t>
+  </si>
+  <si>
+    <t>30508572us</t>
+  </si>
+  <si>
+    <t>219460719us</t>
+  </si>
+  <si>
+    <t>41323us</t>
+  </si>
+  <si>
+    <t>6860153us</t>
+  </si>
+  <si>
+    <t>155523188us</t>
+  </si>
+  <si>
+    <t>68424us</t>
+  </si>
+  <si>
+    <t>21699433us</t>
+  </si>
+  <si>
+    <t>109398us</t>
+  </si>
+  <si>
+    <t>56434399us</t>
+  </si>
+  <si>
+    <t>BACK (n/k)</t>
+  </si>
+  <si>
+    <t>15921us</t>
+  </si>
+  <si>
+    <t>15858us</t>
+  </si>
+  <si>
+    <t>31147us</t>
+  </si>
+  <si>
+    <t>53139us</t>
+  </si>
+  <si>
+    <t>80972us</t>
+  </si>
+  <si>
+    <t>129253us</t>
+  </si>
+  <si>
+    <t>185813us</t>
+  </si>
+  <si>
+    <t>301812us</t>
+  </si>
+  <si>
+    <t>370394us</t>
+  </si>
+  <si>
+    <t>459971us</t>
+  </si>
+  <si>
+    <t>590395us</t>
+  </si>
+  <si>
+    <t>725159us</t>
+  </si>
+  <si>
+    <t>916267us</t>
+  </si>
+  <si>
+    <t>1182489us</t>
+  </si>
+  <si>
+    <t>2546433us</t>
+  </si>
+  <si>
+    <t>8625930us</t>
+  </si>
+  <si>
+    <t>19860930us</t>
+  </si>
+  <si>
+    <t>38335897us</t>
+  </si>
+  <si>
+    <t>302361888us</t>
+  </si>
+  <si>
+    <t>11408us</t>
+  </si>
+  <si>
+    <t>107677us</t>
+  </si>
+  <si>
+    <t>418316us</t>
+  </si>
+  <si>
+    <t>1040470us</t>
+  </si>
+  <si>
+    <t>2511296us</t>
+  </si>
+  <si>
+    <t>4879858us</t>
+  </si>
+  <si>
+    <t>9514172us</t>
+  </si>
+  <si>
+    <t>13756852us</t>
+  </si>
+  <si>
+    <t>20415497us</t>
+  </si>
+  <si>
+    <t>30507460us</t>
+  </si>
+  <si>
+    <t>44123774us</t>
+  </si>
+  <si>
+    <t>61802745us</t>
+  </si>
+  <si>
+    <t>86062011us</t>
+  </si>
+  <si>
+    <t>112302171us</t>
+  </si>
+  <si>
+    <t>63907us</t>
+  </si>
+  <si>
+    <t>1097244us</t>
+  </si>
+  <si>
+    <t>6486246us</t>
+  </si>
+  <si>
+    <t>23403730us</t>
+  </si>
+  <si>
+    <t>63904671us</t>
+  </si>
+  <si>
+    <t>151121120us</t>
+  </si>
+  <si>
+    <t>253336us</t>
+  </si>
+  <si>
+    <t>8249560us</t>
+  </si>
+  <si>
+    <t>71378754us</t>
+  </si>
+  <si>
+    <t>804871us</t>
+  </si>
+  <si>
+    <t>64306006us</t>
+  </si>
+  <si>
+    <t>2017172us</t>
+  </si>
+  <si>
+    <t>4234516us</t>
+  </si>
+  <si>
+    <t>7719329us</t>
+  </si>
+  <si>
+    <t>FILT(n/k)</t>
+  </si>
+  <si>
+    <t>44us</t>
+  </si>
+  <si>
+    <t>120us</t>
+  </si>
+  <si>
+    <t>772us</t>
+  </si>
+  <si>
+    <t>2158us</t>
+  </si>
+  <si>
+    <t>8331us</t>
+  </si>
+  <si>
+    <t>31473us</t>
+  </si>
+  <si>
+    <t>114816us</t>
+  </si>
+  <si>
+    <t>451968us</t>
+  </si>
+  <si>
+    <t>1884762us</t>
+  </si>
+  <si>
+    <t>59309970us</t>
+  </si>
+  <si>
+    <t>31059us</t>
+  </si>
+  <si>
+    <t>439157us</t>
+  </si>
+  <si>
+    <t>7527032us</t>
+  </si>
+  <si>
+    <t>111807354us</t>
+  </si>
+  <si>
+    <t>177070us</t>
+  </si>
+  <si>
+    <t>6864927us</t>
+  </si>
+  <si>
+    <t>77448us</t>
+  </si>
+  <si>
+    <t>6684049us</t>
+  </si>
+  <si>
+    <t>3261us</t>
+  </si>
+  <si>
+    <t>692734us</t>
+  </si>
+  <si>
+    <t>111206117us</t>
+  </si>
+  <si>
+    <t>35us</t>
+  </si>
+  <si>
+    <t>18956us</t>
+  </si>
+  <si>
+    <t>4976471us</t>
+  </si>
+  <si>
+    <t>113us</t>
+  </si>
+  <si>
+    <t>59349us</t>
+  </si>
+  <si>
+    <t>27892493us</t>
+  </si>
+  <si>
+    <t>115us</t>
+  </si>
+  <si>
+    <t>156975us</t>
+  </si>
+  <si>
+    <t>129192183us</t>
+  </si>
+  <si>
+    <t>194us</t>
+  </si>
+  <si>
+    <t>417125us</t>
+  </si>
+  <si>
+    <t>486369392us</t>
+  </si>
+  <si>
+    <t>328us</t>
+  </si>
+  <si>
+    <t>863197us</t>
+  </si>
+  <si>
+    <t>10795us</t>
+  </si>
+  <si>
+    <t>47816us</t>
+  </si>
+  <si>
+    <t>127736us</t>
+  </si>
+  <si>
+    <t>481660us</t>
+  </si>
+  <si>
+    <t>2145556us</t>
+  </si>
+  <si>
+    <t>BACK(n/k)</t>
+  </si>
+  <si>
+    <t>16090670us</t>
+  </si>
+  <si>
+    <t>8924367us</t>
+  </si>
+  <si>
+    <t>1878889us</t>
+  </si>
+  <si>
+    <t>16997us</t>
+  </si>
+  <si>
+    <t>10400393us</t>
+  </si>
+  <si>
+    <t>40926us</t>
+  </si>
+  <si>
+    <t>166203728us</t>
+  </si>
+  <si>
+    <t>189172us</t>
+  </si>
+  <si>
+    <t>152254us</t>
+  </si>
+  <si>
+    <t>289257us</t>
   </si>
 </sst>
 </file>
@@ -273,7 +829,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,18 +838,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -301,19 +863,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -643,388 +1258,1966 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
-  <dimension ref="B2:J25"/>
+  <dimension ref="B2:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>7</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>8</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>9</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="L2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="1">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1">
+        <v>9</v>
+      </c>
+      <c r="T2" s="1">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="W2" s="1">
+        <v>3</v>
+      </c>
+      <c r="X2" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="1">
+        <v>100</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="V3" s="1">
+        <v>100</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
         <v>200</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="G4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="1">
+        <v>200</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="V4" s="1">
+        <v>200</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>300</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="G5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="1">
+        <v>300</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V5" s="1">
+        <v>300</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <v>400</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="G6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="1">
+        <v>400</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="V6" s="1">
+        <v>400</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
         <v>500</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="G7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="L7" s="1">
+        <v>500</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="V7" s="1">
+        <v>500</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>600</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="G8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="L8" s="1">
+        <v>600</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="1">
+        <v>600</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>700</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="G9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="L9" s="1">
+        <v>700</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="V9" s="1">
+        <v>700</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <v>800</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="G10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="L10" s="1">
+        <v>800</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="V10" s="1">
+        <v>800</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>900</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="1">
+        <v>900</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="V11" s="1">
+        <v>900</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="V12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <v>1100</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="L13" s="1">
+        <v>1100</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="V13" s="1">
+        <v>1100</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
         <v>1200</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="F14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="L14" s="1">
+        <v>1200</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="V14" s="1">
+        <v>1200</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
         <v>1300</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="F15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="L15" s="1">
+        <v>1300</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="V15" s="1">
+        <v>1300</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <v>1400</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="F16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="L16" s="1">
+        <v>1400</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="V16" s="1">
+        <v>1400</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>1500</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="L17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="V17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="L18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="V18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>3000</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="L19" s="1">
+        <v>3000</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="V19" s="1">
+        <v>3000</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <v>4000</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="L20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="V20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="L21" s="1">
+        <v>5000</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="V21" s="1">
+        <v>5000</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>10000</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="L22" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="V22" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>20000</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="L23" s="1">
+        <v>20000</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="V23" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>30000</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="L24" s="1">
+        <v>30000</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="V24" s="1">
+        <v>30000</v>
+      </c>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>40000</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="L25" s="1">
+        <v>40000</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="V25" s="1">
+        <v>40000</v>
+      </c>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
+  <dimension ref="B2:X14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1">
+        <v>10</v>
+      </c>
+      <c r="T2" s="1">
+        <v>12</v>
+      </c>
+      <c r="U2" s="1">
+        <v>14</v>
+      </c>
+      <c r="V2" s="1">
+        <v>16</v>
+      </c>
+      <c r="W2" s="1">
+        <v>18</v>
+      </c>
+      <c r="X2" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="N3" s="1">
+        <v>14</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="N4" s="1">
+        <v>16</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="N5" s="1">
+        <v>18</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="N6" s="1">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="N7" s="1">
+        <v>22</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="N8" s="1">
+        <v>24</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="1">
+        <v>26</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="N10" s="1">
+        <v>28</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="1">
+        <v>30</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="1">
+        <v>35</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="1">
+        <v>40</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="N14" s="1">
+        <v>50</v>
+      </c>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Benchmarked inverse k for integer partitions.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B4161C-7E30-47BC-8761-49FAE256D8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE315DE7-A8DC-4CC0-955F-C03FBA89516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="357">
   <si>
     <t>TREE (n/k)</t>
   </si>
@@ -850,6 +850,264 @@
   </si>
   <si>
     <t>3845884us</t>
+  </si>
+  <si>
+    <t>4us</t>
+  </si>
+  <si>
+    <t>1us</t>
+  </si>
+  <si>
+    <t>2us</t>
+  </si>
+  <si>
+    <t>3us</t>
+  </si>
+  <si>
+    <t>15us</t>
+  </si>
+  <si>
+    <t>21us</t>
+  </si>
+  <si>
+    <t>20us</t>
+  </si>
+  <si>
+    <t>60us</t>
+  </si>
+  <si>
+    <t>118us</t>
+  </si>
+  <si>
+    <t>158us</t>
+  </si>
+  <si>
+    <t>252us</t>
+  </si>
+  <si>
+    <t>0us</t>
+  </si>
+  <si>
+    <t>16us</t>
+  </si>
+  <si>
+    <t>29us</t>
+  </si>
+  <si>
+    <t>22us</t>
+  </si>
+  <si>
+    <t>12us</t>
+  </si>
+  <si>
+    <t>64us</t>
+  </si>
+  <si>
+    <t>143us</t>
+  </si>
+  <si>
+    <t>225us</t>
+  </si>
+  <si>
+    <t>235us</t>
+  </si>
+  <si>
+    <t>24us</t>
+  </si>
+  <si>
+    <t>13us</t>
+  </si>
+  <si>
+    <t>162us</t>
+  </si>
+  <si>
+    <t>195us</t>
+  </si>
+  <si>
+    <t>105us</t>
+  </si>
+  <si>
+    <t>5us</t>
+  </si>
+  <si>
+    <t>6us</t>
+  </si>
+  <si>
+    <t>19us</t>
+  </si>
+  <si>
+    <t>26us</t>
+  </si>
+  <si>
+    <t>408us</t>
+  </si>
+  <si>
+    <t>1069us</t>
+  </si>
+  <si>
+    <t>1379us</t>
+  </si>
+  <si>
+    <t>2658us</t>
+  </si>
+  <si>
+    <t>3160us</t>
+  </si>
+  <si>
+    <t>3782us</t>
+  </si>
+  <si>
+    <t>9992us</t>
+  </si>
+  <si>
+    <t>8253us</t>
+  </si>
+  <si>
+    <t>8006us</t>
+  </si>
+  <si>
+    <t>10040us</t>
+  </si>
+  <si>
+    <t>10552us</t>
+  </si>
+  <si>
+    <t>16275us</t>
+  </si>
+  <si>
+    <t>28622us</t>
+  </si>
+  <si>
+    <t>82996us</t>
+  </si>
+  <si>
+    <t>21342us</t>
+  </si>
+  <si>
+    <t>34721us</t>
+  </si>
+  <si>
+    <t>89032us</t>
+  </si>
+  <si>
+    <t>143423us</t>
+  </si>
+  <si>
+    <t>211673us</t>
+  </si>
+  <si>
+    <t>316us</t>
+  </si>
+  <si>
+    <t>696us</t>
+  </si>
+  <si>
+    <t>1410us</t>
+  </si>
+  <si>
+    <t>4014us</t>
+  </si>
+  <si>
+    <t>3041us</t>
+  </si>
+  <si>
+    <t>6860us</t>
+  </si>
+  <si>
+    <t>5252us</t>
+  </si>
+  <si>
+    <t>7322us</t>
+  </si>
+  <si>
+    <t>8536us</t>
+  </si>
+  <si>
+    <t>12866us</t>
+  </si>
+  <si>
+    <t>9270us</t>
+  </si>
+  <si>
+    <t>19206us</t>
+  </si>
+  <si>
+    <t>17314us</t>
+  </si>
+  <si>
+    <t>19425us</t>
+  </si>
+  <si>
+    <t>23977us</t>
+  </si>
+  <si>
+    <t>27893us</t>
+  </si>
+  <si>
+    <t>61957us</t>
+  </si>
+  <si>
+    <t>98460us</t>
+  </si>
+  <si>
+    <t>148470us</t>
+  </si>
+  <si>
+    <t>265us</t>
+  </si>
+  <si>
+    <t>607us</t>
+  </si>
+  <si>
+    <t>1048us</t>
+  </si>
+  <si>
+    <t>1687us</t>
+  </si>
+  <si>
+    <t>2482us</t>
+  </si>
+  <si>
+    <t>3748us</t>
+  </si>
+  <si>
+    <t>7259us</t>
+  </si>
+  <si>
+    <t>5570us</t>
+  </si>
+  <si>
+    <t>6617us</t>
+  </si>
+  <si>
+    <t>6851us</t>
+  </si>
+  <si>
+    <t>10133us</t>
+  </si>
+  <si>
+    <t>9342us</t>
+  </si>
+  <si>
+    <t>13125us</t>
+  </si>
+  <si>
+    <t>16619us</t>
+  </si>
+  <si>
+    <t>14256us</t>
+  </si>
+  <si>
+    <t>26113us</t>
+  </si>
+  <si>
+    <t>50211us</t>
+  </si>
+  <si>
+    <t>90863us</t>
+  </si>
+  <si>
+    <t>157155us</t>
   </si>
 </sst>
 </file>
@@ -928,14 +1186,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -947,13 +1198,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1331,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,14 +1588,18 @@
     <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="22" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6" customWidth="1"/>
+    <col min="26" max="26" width="5.7109375" customWidth="1"/>
+    <col min="27" max="27" width="6" customWidth="1"/>
     <col min="28" max="28" width="13.85546875" customWidth="1"/>
     <col min="29" max="29" width="11.7109375" customWidth="1"/>
     <col min="30" max="30" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="38" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="41" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" customWidth="1"/>
+    <col min="40" max="40" width="8.85546875" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" customWidth="1"/>
     <col min="42" max="42" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1502,9 +1750,15 @@
       <c r="J3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="N3" s="3" t="s">
         <v>265</v>
       </c>
@@ -1535,9 +1789,15 @@
       <c r="X3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
+      <c r="Y3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>271</v>
+      </c>
       <c r="AB3" s="3" t="s">
         <v>268</v>
       </c>
@@ -1568,9 +1828,15 @@
       <c r="AL3" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
+      <c r="AM3" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>300</v>
+      </c>
       <c r="AP3" s="3" t="s">
         <v>270</v>
       </c>
@@ -1603,9 +1869,15 @@
       <c r="J4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="N4" s="3" t="s">
         <v>266</v>
       </c>
@@ -1636,9 +1908,15 @@
       <c r="X4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
+      <c r="Y4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB4" s="3" t="s">
         <v>267</v>
       </c>
@@ -1669,9 +1947,15 @@
       <c r="AL4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="3"/>
+      <c r="AM4" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="AP4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1704,9 +1988,15 @@
       <c r="J5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N5" s="3" t="s">
         <v>264</v>
       </c>
@@ -1737,9 +2027,15 @@
       <c r="X5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
+      <c r="Y5" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB5" s="3" t="s">
         <v>269</v>
       </c>
@@ -1764,9 +2060,15 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
+      <c r="AM5" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="AP5" s="3"/>
     </row>
     <row r="6" spans="2:42" x14ac:dyDescent="0.25">
@@ -1797,9 +2099,15 @@
       <c r="J6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="N6" s="3" t="s">
         <v>57</v>
       </c>
@@ -1826,9 +2134,15 @@
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
+      <c r="Y6" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>297</v>
+      </c>
       <c r="AB6" s="3" t="s">
         <v>57</v>
       </c>
@@ -1851,9 +2165,15 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
+      <c r="AM6" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="AN6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="AP6" s="3"/>
     </row>
     <row r="7" spans="2:42" x14ac:dyDescent="0.25">
@@ -1882,9 +2202,15 @@
         <v>57</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="P7" s="1">
         <v>500</v>
@@ -1907,9 +2233,15 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
+      <c r="Y7" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB7" s="3"/>
       <c r="AD7" s="1">
         <v>500</v>
@@ -1928,9 +2260,15 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
+      <c r="AM7" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AN7" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO7" s="3" t="s">
+        <v>304</v>
+      </c>
       <c r="AP7" s="3"/>
     </row>
     <row r="8" spans="2:42" x14ac:dyDescent="0.25">
@@ -1957,9 +2295,15 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="P8" s="1">
         <v>600</v>
@@ -1980,9 +2324,15 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="Y8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB8" s="3"/>
       <c r="AD8" s="1">
         <v>600</v>
@@ -2001,9 +2351,15 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
+      <c r="AM8" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="AN8" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="AO8" s="3" t="s">
+        <v>305</v>
+      </c>
       <c r="AP8" s="3"/>
     </row>
     <row r="9" spans="2:42" x14ac:dyDescent="0.25">
@@ -2028,9 +2384,15 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N9" s="3"/>
       <c r="P9" s="1">
         <v>700</v>
@@ -2051,9 +2413,15 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
+      <c r="Y9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB9" s="3"/>
       <c r="AD9" s="1">
         <v>700</v>
@@ -2072,9 +2440,15 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="3"/>
+      <c r="AM9" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="AN9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AO9" s="3" t="s">
+        <v>306</v>
+      </c>
       <c r="AP9" s="3"/>
     </row>
     <row r="10" spans="2:42" x14ac:dyDescent="0.25">
@@ -2099,9 +2473,15 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="N10" s="3"/>
       <c r="P10" s="1">
         <v>800</v>
@@ -2120,9 +2500,15 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
+      <c r="Y10" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB10" s="3"/>
       <c r="AD10" s="1">
         <v>800</v>
@@ -2139,9 +2525,15 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
+      <c r="AM10" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN10" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>307</v>
+      </c>
       <c r="AP10" s="3"/>
     </row>
     <row r="11" spans="2:42" x14ac:dyDescent="0.25">
@@ -2164,9 +2556,15 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N11" s="3"/>
       <c r="P11" s="1">
         <v>900</v>
@@ -2185,9 +2583,15 @@
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
+      <c r="Y11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB11" s="3"/>
       <c r="AD11" s="1">
         <v>900</v>
@@ -2204,9 +2608,15 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="3"/>
+      <c r="AM11" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AN11" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>308</v>
+      </c>
       <c r="AP11" s="3"/>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.25">
@@ -2229,9 +2639,15 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N12" s="3"/>
       <c r="P12" s="1">
         <v>1000</v>
@@ -2250,9 +2666,15 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
+      <c r="Y12" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>298</v>
+      </c>
       <c r="AB12" s="3"/>
       <c r="AD12" s="1">
         <v>1000</v>
@@ -2269,9 +2691,15 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
+      <c r="AM12" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AN12" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AO12" s="3" t="s">
+        <v>309</v>
+      </c>
       <c r="AP12" s="3"/>
     </row>
     <row r="13" spans="2:42" x14ac:dyDescent="0.25">
@@ -2294,9 +2722,15 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>283</v>
+      </c>
       <c r="N13" s="3"/>
       <c r="P13" s="1">
         <v>1100</v>
@@ -2313,9 +2747,15 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
+      <c r="Y13" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB13" s="3"/>
       <c r="AD13" s="1">
         <v>1100</v>
@@ -2332,9 +2772,15 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
-      <c r="AM13" s="3"/>
-      <c r="AN13" s="3"/>
-      <c r="AO13" s="3"/>
+      <c r="AM13" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AN13" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AO13" s="3" t="s">
+        <v>310</v>
+      </c>
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.25">
@@ -2357,9 +2803,15 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="K14" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>275</v>
+      </c>
       <c r="N14" s="3"/>
       <c r="P14" s="1">
         <v>1200</v>
@@ -2376,9 +2828,15 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
+      <c r="Y14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB14" s="3"/>
       <c r="AD14" s="1">
         <v>1200</v>
@@ -2395,9 +2853,15 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
-      <c r="AM14" s="3"/>
-      <c r="AN14" s="3"/>
-      <c r="AO14" s="3"/>
+      <c r="AM14" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:42" x14ac:dyDescent="0.25">
@@ -2420,9 +2884,15 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="N15" s="3"/>
       <c r="P15" s="1">
         <v>1300</v>
@@ -2439,9 +2909,15 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
+      <c r="Y15" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB15" s="3"/>
       <c r="AD15" s="1">
         <v>1300</v>
@@ -2458,9 +2934,15 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
-      <c r="AM15" s="3"/>
-      <c r="AN15" s="3"/>
-      <c r="AO15" s="3"/>
+      <c r="AM15" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:42" x14ac:dyDescent="0.25">
@@ -2483,9 +2965,15 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="N16" s="3"/>
       <c r="P16" s="1">
         <v>1400</v>
@@ -2502,9 +2990,15 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
+      <c r="Y16" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB16" s="3"/>
       <c r="AD16" s="1">
         <v>1400</v>
@@ -2521,9 +3015,15 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
-      <c r="AM16" s="3"/>
-      <c r="AN16" s="3"/>
-      <c r="AO16" s="3"/>
+      <c r="AM16" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="AN16" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AO16" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:42" x14ac:dyDescent="0.25">
@@ -2546,9 +3046,15 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="N17" s="3"/>
       <c r="P17" s="1">
         <v>1500</v>
@@ -2565,9 +3071,15 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
+      <c r="Y17" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="AB17" s="3"/>
       <c r="AD17" s="1">
         <v>1500</v>
@@ -2584,9 +3096,15 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
-      <c r="AM17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AO17" s="3"/>
+      <c r="AM17" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="AN17" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AO17" s="3" t="s">
+        <v>314</v>
+      </c>
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:42" x14ac:dyDescent="0.25">
@@ -2607,9 +3125,15 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="N18" s="3"/>
       <c r="P18" s="1">
         <v>2000</v>
@@ -2626,9 +3150,15 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
+      <c r="Y18" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB18" s="3"/>
       <c r="AD18" s="1">
         <v>2000</v>
@@ -2643,9 +3173,15 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
+      <c r="AM18" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="AN18" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="AO18" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="AP18" s="3"/>
     </row>
     <row r="19" spans="2:42" x14ac:dyDescent="0.25">
@@ -2666,9 +3202,15 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="K19" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>291</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="P19" s="1">
         <v>3000</v>
@@ -2685,9 +3227,15 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
+      <c r="Y19" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB19" s="3"/>
       <c r="AD19" s="1">
         <v>3000</v>
@@ -2702,9 +3250,15 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
-      <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
+      <c r="AM19" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="AN19" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="AO19" s="3" t="s">
+        <v>316</v>
+      </c>
       <c r="AP19" s="3"/>
     </row>
     <row r="20" spans="2:42" x14ac:dyDescent="0.25">
@@ -2725,9 +3279,15 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="K20" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>291</v>
+      </c>
       <c r="N20" s="3"/>
       <c r="P20" s="1">
         <v>4000</v>
@@ -2744,9 +3304,15 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
+      <c r="Y20" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB20" s="3"/>
       <c r="AD20" s="1">
         <v>4000</v>
@@ -2761,9 +3327,15 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
-      <c r="AM20" s="3"/>
-      <c r="AN20" s="3"/>
-      <c r="AO20" s="3"/>
+      <c r="AM20" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AN20" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="AO20" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="AP20" s="3"/>
     </row>
     <row r="21" spans="2:42" x14ac:dyDescent="0.25">
@@ -2782,9 +3354,15 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="K21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="N21" s="3"/>
       <c r="P21" s="1">
         <v>5000</v>
@@ -2799,9 +3377,15 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
+      <c r="Y21" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB21" s="3"/>
       <c r="AD21" s="1">
         <v>5000</v>
@@ -2816,9 +3400,15 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
-      <c r="AM21" s="3"/>
-      <c r="AN21" s="3"/>
-      <c r="AO21" s="3"/>
+      <c r="AM21" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="AN21" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="AO21" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="AP21" s="3"/>
     </row>
     <row r="22" spans="2:42" x14ac:dyDescent="0.25">
@@ -2837,9 +3427,15 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="N22" s="3"/>
       <c r="P22" s="1">
         <v>10000</v>
@@ -2854,9 +3450,15 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
+      <c r="Y22" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="AB22" s="3"/>
       <c r="AD22" s="1">
         <v>10000</v>
@@ -2871,9 +3473,15 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
-      <c r="AO22" s="3"/>
+      <c r="AM22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO22" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:42" x14ac:dyDescent="0.25">
@@ -2892,9 +3500,15 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="K23" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="N23" s="3"/>
       <c r="P23" s="1">
         <v>20000</v>
@@ -2907,9 +3521,15 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
+      <c r="Y23" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="AB23" s="3"/>
       <c r="AD23" s="1">
         <v>20000</v>
@@ -2943,9 +3563,15 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="K24" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="P24" s="1">
         <v>30000</v>
@@ -2958,9 +3584,15 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
+      <c r="Y24" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="AB24" s="3"/>
       <c r="AD24" s="1">
         <v>30000</v>
@@ -2992,9 +3624,15 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="K25" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>295</v>
+      </c>
       <c r="N25" s="3"/>
       <c r="P25" s="1">
         <v>40000</v>
@@ -3007,9 +3645,15 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
+      <c r="Y25" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA25" s="3" t="s">
+        <v>299</v>
+      </c>
       <c r="AB25" s="3"/>
       <c r="AD25" s="1">
         <v>40000</v>
@@ -3029,10 +3673,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3746,13 +4390,13 @@
       <c r="AF14" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A15:XFD1048576 A2:M14 AO2:XFD14 R2:AC14">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:M14 R2:AC14 AO2:XFD14 A15:XFD1048576">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A15:XFD1048576 AO2:XFD14 A2:AF14">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:AF14 AO2:XFD14 A15:XFD1048576">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Benchmarked inverse k for set partitions.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE315DE7-A8DC-4CC0-955F-C03FBA89516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573C9F92-0E0C-4A6E-A57B-0AAAAD3854FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Integer Partitioning" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="418">
   <si>
     <t>TREE (n/k)</t>
   </si>
@@ -1108,6 +1108,189 @@
   </si>
   <si>
     <t>157155us</t>
+  </si>
+  <si>
+    <t>7us</t>
+  </si>
+  <si>
+    <t>10us</t>
+  </si>
+  <si>
+    <t>45us</t>
+  </si>
+  <si>
+    <t>56us</t>
+  </si>
+  <si>
+    <t>175us</t>
+  </si>
+  <si>
+    <t>91us</t>
+  </si>
+  <si>
+    <t>126us</t>
+  </si>
+  <si>
+    <t>189us</t>
+  </si>
+  <si>
+    <t>410us</t>
+  </si>
+  <si>
+    <t>672us</t>
+  </si>
+  <si>
+    <t>1004us</t>
+  </si>
+  <si>
+    <t>1495us</t>
+  </si>
+  <si>
+    <t>2097us</t>
+  </si>
+  <si>
+    <t>4151us</t>
+  </si>
+  <si>
+    <t>8803us</t>
+  </si>
+  <si>
+    <t>31062us</t>
+  </si>
+  <si>
+    <t>436us</t>
+  </si>
+  <si>
+    <t>1792us</t>
+  </si>
+  <si>
+    <t>3134us</t>
+  </si>
+  <si>
+    <t>15162us</t>
+  </si>
+  <si>
+    <t>20911us</t>
+  </si>
+  <si>
+    <t>62361us</t>
+  </si>
+  <si>
+    <t>76187us</t>
+  </si>
+  <si>
+    <t>93257us</t>
+  </si>
+  <si>
+    <t>152464us</t>
+  </si>
+  <si>
+    <t>445788us</t>
+  </si>
+  <si>
+    <t>1089082us</t>
+  </si>
+  <si>
+    <t>5806986us</t>
+  </si>
+  <si>
+    <t>1827us</t>
+  </si>
+  <si>
+    <t>1097us</t>
+  </si>
+  <si>
+    <t>1624us</t>
+  </si>
+  <si>
+    <t>2406us</t>
+  </si>
+  <si>
+    <t>4063us</t>
+  </si>
+  <si>
+    <t>21727us</t>
+  </si>
+  <si>
+    <t>8851us</t>
+  </si>
+  <si>
+    <t>10730us</t>
+  </si>
+  <si>
+    <t>10767us</t>
+  </si>
+  <si>
+    <t>20196us</t>
+  </si>
+  <si>
+    <t>34928us</t>
+  </si>
+  <si>
+    <t>83532us</t>
+  </si>
+  <si>
+    <t>24353us</t>
+  </si>
+  <si>
+    <t>65663us</t>
+  </si>
+  <si>
+    <t>74668us</t>
+  </si>
+  <si>
+    <t>137859us</t>
+  </si>
+  <si>
+    <t>245027us</t>
+  </si>
+  <si>
+    <t>396088us</t>
+  </si>
+  <si>
+    <t>672337us</t>
+  </si>
+  <si>
+    <t>999572us</t>
+  </si>
+  <si>
+    <t>1578376us</t>
+  </si>
+  <si>
+    <t>3833036us</t>
+  </si>
+  <si>
+    <t>9156522us</t>
+  </si>
+  <si>
+    <t>65501637us</t>
+  </si>
+  <si>
+    <t>239193us</t>
+  </si>
+  <si>
+    <t>676641us</t>
+  </si>
+  <si>
+    <t>1793670us</t>
+  </si>
+  <si>
+    <t>4686700us</t>
+  </si>
+  <si>
+    <t>12414109us</t>
+  </si>
+  <si>
+    <t>41274616us</t>
+  </si>
+  <si>
+    <t>263048466us</t>
+  </si>
+  <si>
+    <t>167672us</t>
+  </si>
+  <si>
+    <t>11545300us</t>
   </si>
 </sst>
 </file>
@@ -1575,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ23" sqref="AJ23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3689,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
   <dimension ref="B2:AF14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,6 +3894,8 @@
     <col min="20" max="20" width="11" customWidth="1"/>
     <col min="21" max="21" width="12.140625" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
+    <col min="30" max="30" width="10.28515625" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
@@ -3831,13 +4016,18 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3" t="str">
-        <f>H3</f>
-        <v>35us</v>
-      </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>416</v>
+      </c>
       <c r="R3" s="1">
         <v>14</v>
       </c>
@@ -3863,10 +4053,18 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
+      <c r="AC3" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -3896,13 +4094,18 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3" t="str">
-        <f t="shared" ref="N4:N6" si="0">H4</f>
-        <v>18956us</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="R4" s="1">
         <v>16</v>
       </c>
@@ -3926,9 +4129,15 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AC4" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>410</v>
+      </c>
       <c r="AF4" s="3"/>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.25">
@@ -3961,13 +4170,18 @@
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>4976471us</v>
-      </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="R5" s="1">
         <v>18</v>
       </c>
@@ -3989,9 +4203,15 @@
       </c>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
+      <c r="AC5" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>411</v>
+      </c>
       <c r="AF5" s="3"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
@@ -4022,12 +4242,15 @@
         <v>238</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>TIME</v>
-      </c>
-      <c r="O6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>376</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="R6" s="1">
         <v>20</v>
@@ -4050,9 +4273,15 @@
         <v>257</v>
       </c>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
+      <c r="AC6" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>412</v>
+      </c>
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
@@ -4081,9 +4310,15 @@
       <c r="L7" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>377</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="R7" s="1">
         <v>22</v>
@@ -4104,9 +4339,15 @@
       <c r="AB7" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
+      <c r="AC7" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>413</v>
+      </c>
       <c r="AF7" s="3"/>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.25">
@@ -4131,9 +4372,15 @@
       <c r="L8" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="M8" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>378</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="R8" s="1">
         <v>24</v>
@@ -4152,9 +4399,15 @@
       <c r="AB8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
+      <c r="AC8" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>414</v>
+      </c>
       <c r="AF8" s="3"/>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
@@ -4177,9 +4430,15 @@
       <c r="L9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>379</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="R9" s="1">
         <v>26</v>
@@ -4196,9 +4455,15 @@
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
+      <c r="AC9" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>415</v>
+      </c>
       <c r="AF9" s="3"/>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.25">
@@ -4217,9 +4482,15 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>380</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="R10" s="1">
         <v>28</v>
@@ -4234,9 +4505,15 @@
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
+      <c r="AC10" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="AF10" s="3"/>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.25">
@@ -4255,9 +4532,15 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>381</v>
+      </c>
       <c r="P11" s="3"/>
       <c r="R11" s="1">
         <v>30</v>
@@ -4272,8 +4555,12 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
+      <c r="AC11" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>405</v>
+      </c>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
     </row>
@@ -4293,9 +4580,15 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>382</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="R12" s="1">
         <v>35</v>
@@ -4310,8 +4603,12 @@
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
+      <c r="AC12" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>406</v>
+      </c>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
     </row>
@@ -4331,9 +4628,15 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="M13" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="P13" s="3"/>
       <c r="R13" s="1">
         <v>40</v>
@@ -4348,8 +4651,12 @@
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
+      <c r="AC13" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>407</v>
+      </c>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
     </row>
@@ -4367,9 +4674,15 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>384</v>
+      </c>
       <c r="P14" s="3"/>
       <c r="R14" s="1">
         <v>50</v>
@@ -4384,8 +4697,12 @@
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="AC14" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>408</v>
+      </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fixed the counting script for integers.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1B3840-343A-418A-B822-3B6CB3FE5EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F250D01-D266-45B1-9091-0196F6201092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -144,31 +144,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -186,14 +176,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -529,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AP50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +547,7 @@
     <col min="42" max="42" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -598,396 +588,1262 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="C3" s="2">
+        <v>850</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7361</v>
+      </c>
+      <c r="E3" s="2">
+        <v>39744</v>
+      </c>
+      <c r="F3" s="2">
+        <v>150224</v>
+      </c>
+      <c r="G3" s="2">
+        <v>430768</v>
+      </c>
+      <c r="H3" s="2">
+        <v>992250</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1918204</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3218412</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="3">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>7</v>
+      </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>200</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="C4" s="2">
+        <v>3367</v>
+      </c>
+      <c r="D4" s="2">
+        <v>57222</v>
+      </c>
+      <c r="E4" s="2">
+        <v>595085</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4234086</v>
+      </c>
+      <c r="G4" s="2">
+        <v>22225872</v>
+      </c>
+      <c r="H4" s="2">
+        <v>90894094</v>
+      </c>
+      <c r="I4" s="2">
+        <v>301883042</v>
+      </c>
+      <c r="J4" s="2">
+        <v>841359596</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>7</v>
+      </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>300</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="C5" s="2">
+        <v>7550</v>
+      </c>
+      <c r="D5" s="2">
+        <v>191250</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2945190</v>
+      </c>
+      <c r="F5" s="2">
+        <v>30774260</v>
+      </c>
+      <c r="G5" s="2">
+        <v>234822553</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1379643821</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6497669574</v>
+      </c>
+      <c r="J5" s="2">
+        <v>25322313307</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3">
+        <v>5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>7</v>
+      </c>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>400</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="C6" s="2">
+        <v>13400</v>
+      </c>
+      <c r="D6" s="2">
+        <v>451111</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9202559</v>
+      </c>
+      <c r="F6" s="2">
+        <v>126835109</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1269817428</v>
+      </c>
+      <c r="H6" s="2">
+        <v>9727994039</v>
+      </c>
+      <c r="I6" s="2">
+        <v>59323995199</v>
+      </c>
+      <c r="J6" s="2">
+        <v>297074585225</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7</v>
+      </c>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>500</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="C7" s="2">
+        <v>20917</v>
+      </c>
+      <c r="D7" s="2">
+        <v>878472</v>
+      </c>
+      <c r="E7" s="2">
+        <v>22313025</v>
+      </c>
+      <c r="F7" s="2">
+        <v>381911546</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4732871282</v>
+      </c>
+      <c r="H7" s="2">
+        <v>44709647908</v>
+      </c>
+      <c r="I7" s="2">
+        <v>334740200089</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2048073072881</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>7</v>
+      </c>
       <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>600</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="C8" s="2">
+        <v>30100</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1515000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>46055755</v>
+      </c>
+      <c r="F8" s="2">
+        <v>941817895</v>
+      </c>
+      <c r="G8" s="2">
+        <v>13914026520</v>
+      </c>
+      <c r="H8" s="2">
+        <v>156286689060</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1387159599492</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10028114108467</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5</v>
+      </c>
+      <c r="M8" s="3">
+        <v>7</v>
+      </c>
       <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>700</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="C9" s="2">
+        <v>40950</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2402361</v>
+      </c>
+      <c r="E9" s="2">
+        <v>85043249</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2022576869</v>
+      </c>
+      <c r="G9" s="2">
+        <v>34696437288</v>
+      </c>
+      <c r="H9" s="2">
+        <v>451678463853</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4636266938051</v>
+      </c>
+      <c r="J9" s="2">
+        <v>38667208407883</v>
+      </c>
+      <c r="K9" s="3">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>5</v>
+      </c>
+      <c r="M9" s="3">
+        <v>7</v>
+      </c>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>800</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="C10" s="2">
+        <v>53467</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3582222</v>
+      </c>
+      <c r="E10" s="2">
+        <v>144721340</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3924308381</v>
+      </c>
+      <c r="G10" s="2">
+        <v>76663512392</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1134904074747</v>
+      </c>
+      <c r="I10" s="2">
+        <v>13225427691101</v>
+      </c>
+      <c r="J10" s="2">
+        <v>124995134376940</v>
+      </c>
+      <c r="K10" s="3">
+        <v>3</v>
+      </c>
+      <c r="L10" s="3">
+        <v>5</v>
+      </c>
+      <c r="M10" s="3">
+        <v>7</v>
+      </c>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>900</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="C11" s="3">
+        <v>67650</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5096250</v>
+      </c>
+      <c r="E11" s="3">
+        <v>231369195</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7045118405</v>
+      </c>
+      <c r="G11" s="3">
+        <v>154404470830</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2561478643574</v>
+      </c>
+      <c r="I11" s="3">
+        <v>33407250281517</v>
+      </c>
+      <c r="J11" s="3">
+        <v>352851241223889</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>7</v>
+      </c>
       <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="7"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="C12" s="3">
+        <v>83500</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6986111</v>
+      </c>
+      <c r="E12" s="3">
+        <v>352099314</v>
+      </c>
+      <c r="F12" s="3">
+        <v>11894988004</v>
+      </c>
+      <c r="G12" s="3">
+        <v>289018309991</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5310743503299</v>
+      </c>
+      <c r="I12" s="3">
+        <v>76639419601247</v>
+      </c>
+      <c r="J12" s="3">
+        <v>894622011523232</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5</v>
+      </c>
+      <c r="M12" s="3">
+        <v>7</v>
+      </c>
       <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="7"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>1100</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="C13" s="3">
+        <v>101017</v>
+      </c>
+      <c r="D13" s="3">
+        <v>9293472</v>
+      </c>
+      <c r="E13" s="3">
+        <v>514857530</v>
+      </c>
+      <c r="F13" s="3">
+        <v>19109662091</v>
+      </c>
+      <c r="G13" s="3">
+        <v>509816186702</v>
+      </c>
+      <c r="H13" s="3">
+        <v>10278310477111</v>
+      </c>
+      <c r="I13" s="3">
+        <v>162601477536085</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2078723886265530</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>5</v>
+      </c>
+      <c r="M13" s="3">
+        <v>7</v>
+      </c>
       <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="7"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1200</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="C14" s="3">
+        <v>120200</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12060000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>728423010</v>
+      </c>
+      <c r="F14" s="3">
+        <v>29464538290</v>
+      </c>
+      <c r="G14" s="3">
+        <v>856222210840</v>
+      </c>
+      <c r="H14" s="3">
+        <v>18791100403613</v>
+      </c>
+      <c r="I14" s="3">
+        <v>323370783523261</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4493304421998500</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3">
+        <v>5</v>
+      </c>
+      <c r="M14" s="3">
+        <v>7</v>
+      </c>
       <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="7"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1300</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="C15" s="3">
+        <v>141050</v>
+      </c>
+      <c r="D15" s="3">
+        <v>15327361</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1002408254</v>
+      </c>
+      <c r="F15" s="3">
+        <v>43888556014</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1379872651608</v>
+      </c>
+      <c r="H15" s="3">
+        <v>32747456066663</v>
+      </c>
+      <c r="I15" s="3">
+        <v>609023445489943</v>
+      </c>
+      <c r="J15" s="3">
+        <v>9139165989440510</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3">
+        <v>5</v>
+      </c>
+      <c r="M15" s="3">
+        <v>7</v>
+      </c>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="7"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1400</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="C16" s="3">
+        <v>163567</v>
+      </c>
+      <c r="D16" s="3">
+        <v>19137222</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1347259095</v>
+      </c>
+      <c r="F16" s="3">
+        <v>63478085176</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2146913556712</v>
+      </c>
+      <c r="H16" s="8">
+        <v>54784809688750</v>
+      </c>
+      <c r="I16" s="8">
+        <v>1094953568823150</v>
+      </c>
+      <c r="J16" s="8">
+        <v>1.7647722935916E+16</v>
+      </c>
+      <c r="K16" s="8">
+        <v>3</v>
+      </c>
+      <c r="L16" s="8">
+        <v>5</v>
+      </c>
+      <c r="M16" s="8">
+        <v>7</v>
+      </c>
       <c r="N16" s="3"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
     </row>
     <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1500</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="C17" s="3">
+        <v>187750</v>
+      </c>
+      <c r="D17" s="3">
+        <v>23531250</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1774254700</v>
+      </c>
+      <c r="F17" s="3">
+        <v>89510815050</v>
+      </c>
+      <c r="G17" s="8">
+        <v>3240496784050</v>
+      </c>
+      <c r="H17" s="8">
+        <v>88477385146677</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1891231728363360</v>
+      </c>
+      <c r="J17" s="8">
+        <v>3.25828854201028E+16</v>
+      </c>
+      <c r="K17" s="8">
+        <v>3</v>
+      </c>
+      <c r="L17" s="8">
+        <v>5</v>
+      </c>
+      <c r="M17" s="8">
+        <v>7</v>
+      </c>
       <c r="N17" s="3"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
     </row>
     <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="C18" s="3">
+        <v>333667</v>
+      </c>
+      <c r="D18" s="3">
+        <v>55722222</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5594508350</v>
+      </c>
+      <c r="F18" s="3">
+        <v>375483964471</v>
+      </c>
+      <c r="G18" s="8">
+        <v>18063436158832</v>
+      </c>
+      <c r="H18" s="8">
+        <v>654478064673960</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1.85346098736255E+16</v>
+      </c>
+      <c r="J18" s="8">
+        <v>4.2228883290359802E+17</v>
+      </c>
+      <c r="K18" s="8">
+        <v>3</v>
+      </c>
+      <c r="L18" s="8">
+        <v>5</v>
+      </c>
+      <c r="M18" s="8">
+        <v>7</v>
+      </c>
       <c r="N18" s="3"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
     </row>
     <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>3000</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="C19" s="3">
+        <v>750500</v>
+      </c>
+      <c r="D19" s="3">
+        <v>187875000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>28256393775</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2838352114475</v>
+      </c>
+      <c r="G19" s="8">
+        <v>204124699710600</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1.10409673891502E+16</v>
+      </c>
+      <c r="I19" s="8">
+        <v>4.6602258787669702E+17</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1.5795722712310901E+19</v>
+      </c>
+      <c r="K19" s="8">
+        <v>3</v>
+      </c>
+      <c r="L19" s="8">
+        <v>5</v>
+      </c>
+      <c r="M19" s="8">
+        <v>7</v>
+      </c>
       <c r="N19" s="3"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="6"/>
+      <c r="AK19" s="6"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="6"/>
     </row>
     <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4000</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="C20" s="3">
+        <v>1334000</v>
+      </c>
+      <c r="D20" s="3">
+        <v>445111111</v>
+      </c>
+      <c r="E20" s="3">
+        <v>89200255589</v>
+      </c>
+      <c r="F20" s="3">
+        <v>11933501289979</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1142348229996940</v>
+      </c>
+      <c r="H20" s="8">
+        <v>8.2187910023853408E+16</v>
+      </c>
+      <c r="I20" s="8">
+        <v>4.6105233020709202E+18</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2.0750025041541399E+20</v>
+      </c>
+      <c r="K20" s="8">
+        <v>3</v>
+      </c>
+      <c r="L20" s="8">
+        <v>5</v>
+      </c>
+      <c r="M20" s="8">
+        <v>7</v>
+      </c>
       <c r="N20" s="3"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="6"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="C21" s="3">
+        <v>2084167</v>
+      </c>
+      <c r="D21" s="3">
+        <v>869097222</v>
+      </c>
+      <c r="E21" s="3">
+        <v>217621927125</v>
+      </c>
+      <c r="F21" s="3">
+        <v>36368238898446</v>
+      </c>
+      <c r="G21" s="8">
+        <v>4347302470536430</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3.9040339416227802E+17</v>
+      </c>
+      <c r="I21" s="8">
+        <v>2.7322852856004698E+19</v>
+      </c>
+      <c r="J21" s="8">
+        <v>1.533272596169E+21</v>
+      </c>
+      <c r="K21" s="8">
+        <v>3</v>
+      </c>
+      <c r="L21" s="8">
+        <v>5</v>
+      </c>
+      <c r="M21" s="8">
+        <v>7</v>
+      </c>
       <c r="N21" s="3"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
     </row>
     <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>10000</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="C22" s="3">
+        <v>8335000</v>
+      </c>
+      <c r="D22" s="3">
+        <v>6948611111</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3477084930639</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1160592901581420</v>
+      </c>
+      <c r="G22" s="8">
+        <v>2.7689810809092E+17</v>
+      </c>
+      <c r="H22" s="8">
+        <v>4.9589487815766499E+19</v>
+      </c>
+      <c r="I22" s="8">
+        <v>6.9142922330439303E+21</v>
+      </c>
+      <c r="J22" s="8">
+        <v>7.7213503618299507E+23</v>
+      </c>
+      <c r="K22" s="8">
+        <v>3</v>
+      </c>
+      <c r="L22" s="8">
+        <v>5</v>
+      </c>
+      <c r="M22" s="8">
+        <v>7</v>
+      </c>
       <c r="N22" s="3"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="6"/>
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="6"/>
     </row>
     <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>20000</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="C23" s="3">
+        <v>33336667</v>
+      </c>
+      <c r="D23" s="3">
+        <v>55572222222</v>
+      </c>
+      <c r="E23" s="3">
+        <v>55594450833500</v>
+      </c>
+      <c r="F23" s="3">
+        <v>3.70879839520058E+16</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1.7679046967901499E+19</v>
+      </c>
+      <c r="H23" s="8">
+        <v>6.3231006763002196E+21</v>
+      </c>
+      <c r="I23" s="8">
+        <v>1.7598420206522899E+24</v>
+      </c>
+      <c r="J23" s="8">
+        <v>3.9206355537377398E+26</v>
+      </c>
+      <c r="K23" s="8">
+        <v>3</v>
+      </c>
+      <c r="L23" s="8">
+        <v>5</v>
+      </c>
+      <c r="M23" s="8">
+        <v>7</v>
+      </c>
       <c r="N23" s="3"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="6"/>
+      <c r="AK23" s="6"/>
+      <c r="AL23" s="6"/>
+      <c r="AM23" s="6"/>
     </row>
     <row r="24" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>30000</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="C24" s="3">
+        <v>75005000</v>
+      </c>
+      <c r="D24" s="3">
+        <v>187537500000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>281381264375250</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2.8150788333645699E+17</v>
+      </c>
+      <c r="G24" s="8">
+        <v>2.01214460972024E+20</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1.07897662416109E+23</v>
+      </c>
+      <c r="I24" s="8">
+        <v>4.5015805652279704E+25</v>
+      </c>
+      <c r="J24" s="8">
+        <v>1.50305288509519E+28</v>
+      </c>
+      <c r="K24" s="8">
+        <v>3</v>
+      </c>
+      <c r="L24" s="8">
+        <v>5</v>
+      </c>
+      <c r="M24" s="8">
+        <v>7</v>
+      </c>
       <c r="N24" s="3"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="6"/>
+      <c r="AK24" s="6"/>
+      <c r="AL24" s="6"/>
+      <c r="AM24" s="6"/>
     </row>
     <row r="25" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>40000</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="C25" s="3">
+        <v>133340000</v>
+      </c>
+      <c r="D25" s="3">
+        <v>444511111111</v>
+      </c>
+      <c r="E25" s="3">
+        <v>889200025555889</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1.1860001679067799E+18</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1.13010284664268E+21</v>
+      </c>
+      <c r="H25" s="8">
+        <v>8.0780155438337898E+23</v>
+      </c>
+      <c r="I25" s="8">
+        <v>4.4921621030273502E+26</v>
+      </c>
+      <c r="J25" s="8">
+        <v>1.9990371994829001E+29</v>
+      </c>
+      <c r="K25" s="8">
+        <v>3</v>
+      </c>
+      <c r="L25" s="8">
+        <v>5</v>
+      </c>
+      <c r="M25" s="8">
+        <v>7</v>
+      </c>
       <c r="N25" s="3"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
     </row>
     <row r="27" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -3846,19 +4702,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A56:XFD1048576 A2:A55 AT2:XFD55 B27:AS55">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:A55 AT2:XFD55 B27:AS55 A56:XFD1048576 B2:N2 S14:AB14 B3:B25 Q14:Q15 N14:N25 Y23:AB25 Q17:Q25 R15:X25 C3 K11:M14 E3:M3 C4:M10">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"CRASH"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:N25">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"TIME"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5054,13 +5902,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:XFD1048576 A2:M14 R2:AC14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:M14 R2:AC14 AO2:XFD14 A15:XFD1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:XFD1048576 A2:AF14">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 A2:AF14 AO2:XFD14 A15:XFD1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed the counting script for integers again.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F250D01-D266-45B1-9091-0196F6201092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E631A084-D210-461A-87B8-15CCDAA21DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -153,7 +153,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
-  <dimension ref="B2:AP50"/>
+  <dimension ref="B2:AT50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +546,7 @@
     <col min="42" max="42" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -587,299 +586,784 @@
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="X2">
+        <v>833</v>
+      </c>
+      <c r="Y2">
+        <v>3333</v>
+      </c>
+      <c r="Z2">
+        <v>7500</v>
+      </c>
+      <c r="AA2">
+        <v>13333</v>
+      </c>
+      <c r="AB2">
+        <v>20833</v>
+      </c>
+      <c r="AC2">
+        <v>30000</v>
+      </c>
+      <c r="AD2">
+        <v>40833</v>
+      </c>
+      <c r="AE2">
+        <v>53333</v>
+      </c>
+      <c r="AF2">
+        <v>67500</v>
+      </c>
+      <c r="AG2">
+        <v>83333</v>
+      </c>
+      <c r="AH2">
+        <v>100833</v>
+      </c>
+      <c r="AI2">
+        <v>120000</v>
+      </c>
+      <c r="AJ2">
+        <v>140833</v>
+      </c>
+      <c r="AK2">
+        <v>163333</v>
+      </c>
+      <c r="AL2">
+        <v>187500</v>
+      </c>
+      <c r="AM2">
+        <v>333333</v>
+      </c>
+      <c r="AN2">
+        <v>750000</v>
+      </c>
+      <c r="AO2">
+        <v>1333333</v>
+      </c>
+      <c r="AP2">
+        <v>2083333</v>
+      </c>
+      <c r="AQ2">
+        <v>8333333</v>
+      </c>
+      <c r="AR2">
+        <v>33333333</v>
+      </c>
+      <c r="AS2">
+        <v>75000000</v>
+      </c>
+      <c r="AT2">
+        <v>133333333</v>
+      </c>
     </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="2">
-        <v>850</v>
-      </c>
-      <c r="D3" s="3">
-        <v>7361</v>
-      </c>
-      <c r="E3" s="2">
-        <v>39744</v>
-      </c>
-      <c r="F3" s="2">
-        <v>150224</v>
-      </c>
-      <c r="G3" s="2">
-        <v>430768</v>
-      </c>
-      <c r="H3" s="2">
-        <v>992250</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1918204</v>
-      </c>
-      <c r="J3" s="2">
-        <v>3218412</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="C3">
+        <v>833</v>
+      </c>
+      <c r="D3" s="7">
+        <v>7153</v>
+      </c>
+      <c r="E3">
+        <v>38225</v>
+      </c>
+      <c r="F3">
+        <v>143247</v>
+      </c>
+      <c r="G3">
+        <v>407254</v>
+      </c>
+      <c r="H3">
+        <v>930912</v>
+      </c>
+      <c r="I3">
+        <v>1786528</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2977866</v>
+      </c>
+      <c r="K3" s="6">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6">
         <v>3</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="6">
         <v>5</v>
       </c>
-      <c r="M3" s="3">
-        <v>7</v>
-      </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="6">
+        <v>204226</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7">
+        <v>7153</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>56389</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>189375</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>447778</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>873264</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>1507500</v>
+      </c>
+      <c r="AD3">
+        <v>2392153</v>
+      </c>
+      <c r="AE3">
+        <v>3568889</v>
+      </c>
+      <c r="AF3">
+        <v>5079375</v>
+      </c>
+      <c r="AG3">
+        <v>6965278</v>
+      </c>
+      <c r="AH3">
+        <v>9268264</v>
+      </c>
+      <c r="AI3">
+        <v>12030000</v>
+      </c>
+      <c r="AJ3">
+        <v>15292153</v>
+      </c>
+      <c r="AK3">
+        <v>19096389</v>
+      </c>
+      <c r="AL3">
+        <v>23484375</v>
+      </c>
+      <c r="AM3">
+        <v>55638889</v>
+      </c>
+      <c r="AN3">
+        <v>187687500</v>
+      </c>
+      <c r="AO3">
+        <v>444777778</v>
+      </c>
+      <c r="AP3">
+        <v>868576389</v>
+      </c>
+      <c r="AQ3">
+        <v>6946527778</v>
+      </c>
+      <c r="AR3">
+        <v>55563888889</v>
+      </c>
+      <c r="AS3">
+        <v>187518750000</v>
+      </c>
+      <c r="AT3">
+        <v>444477777778</v>
+      </c>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>200</v>
       </c>
-      <c r="C4" s="2">
-        <v>3367</v>
-      </c>
-      <c r="D4" s="2">
-        <v>57222</v>
-      </c>
-      <c r="E4" s="2">
-        <v>595085</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4234086</v>
-      </c>
-      <c r="G4" s="2">
-        <v>22225872</v>
-      </c>
-      <c r="H4" s="2">
-        <v>90894094</v>
-      </c>
-      <c r="I4" s="2">
-        <v>301883042</v>
-      </c>
-      <c r="J4" s="2">
-        <v>841359596</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="C4">
+        <v>3333</v>
+      </c>
+      <c r="D4" s="6">
+        <v>56389</v>
+      </c>
+      <c r="E4">
+        <v>583464</v>
+      </c>
+      <c r="F4">
+        <v>4132096</v>
+      </c>
+      <c r="G4">
+        <v>21591496</v>
+      </c>
+      <c r="H4">
+        <v>87914929</v>
+      </c>
+      <c r="I4">
+        <v>290766028</v>
+      </c>
+      <c r="J4" s="7">
+        <v>807151588</v>
+      </c>
+      <c r="K4" s="6">
+        <v>2</v>
+      </c>
+      <c r="L4" s="6">
         <v>3</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="6">
         <v>5</v>
       </c>
-      <c r="M4" s="3">
-        <v>7</v>
-      </c>
-      <c r="N4" s="3"/>
+      <c r="N4" s="6">
+        <v>190569292</v>
+      </c>
+      <c r="X4">
+        <v>38225</v>
+      </c>
+      <c r="Y4">
+        <v>583464</v>
+      </c>
+      <c r="Z4">
+        <v>2906550</v>
+      </c>
+      <c r="AA4">
+        <v>9111650</v>
+      </c>
+      <c r="AB4">
+        <v>22136264</v>
+      </c>
+      <c r="AC4">
+        <v>45751225</v>
+      </c>
+      <c r="AD4">
+        <v>84560700</v>
+      </c>
+      <c r="AE4">
+        <v>144002189</v>
+      </c>
+      <c r="AF4">
+        <v>230346525</v>
+      </c>
+      <c r="AG4">
+        <v>350697875</v>
+      </c>
+      <c r="AH4">
+        <v>512993739</v>
+      </c>
+      <c r="AI4">
+        <v>726004950</v>
+      </c>
+      <c r="AJ4">
+        <v>999335675</v>
+      </c>
+      <c r="AK4">
+        <v>1343423414</v>
+      </c>
+      <c r="AL4">
+        <v>1769539000</v>
+      </c>
+      <c r="AM4">
+        <v>5583347139</v>
+      </c>
+      <c r="AN4">
+        <v>28218781125</v>
+      </c>
+      <c r="AO4">
+        <v>89111166500</v>
+      </c>
+      <c r="AP4">
+        <v>217448003264</v>
+      </c>
+      <c r="AQ4">
+        <v>3475694791250</v>
+      </c>
+      <c r="AR4">
+        <v>55583334721389</v>
+      </c>
+      <c r="AS4">
+        <v>281343753123750</v>
+      </c>
+      <c r="AT4">
+        <v>889111116665000</v>
+      </c>
     </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>300</v>
       </c>
-      <c r="C5" s="2">
-        <v>7550</v>
-      </c>
-      <c r="D5" s="2">
-        <v>191250</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2945190</v>
-      </c>
-      <c r="F5" s="2">
-        <v>30774260</v>
-      </c>
-      <c r="G5" s="2">
-        <v>234822553</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1379643821</v>
-      </c>
-      <c r="I5" s="2">
-        <v>6497669574</v>
-      </c>
-      <c r="J5" s="2">
-        <v>25322313307</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="C5">
+        <v>7500</v>
+      </c>
+      <c r="D5" s="6">
+        <v>189375</v>
+      </c>
+      <c r="E5">
+        <v>2906550</v>
+      </c>
+      <c r="F5" s="5">
+        <v>30273960</v>
+      </c>
+      <c r="G5" s="5">
+        <v>230282157</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1348858067</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6333941094</v>
+      </c>
+      <c r="J5" s="6">
+        <v>24613920986</v>
+      </c>
+      <c r="K5" s="6">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6">
         <v>3</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="6">
         <v>5</v>
       </c>
-      <c r="M5" s="3">
-        <v>7</v>
-      </c>
-      <c r="N5" s="3"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
+      <c r="N5" s="6">
+        <v>40853235313</v>
+      </c>
+      <c r="X5">
+        <v>143247</v>
+      </c>
+      <c r="Y5">
+        <v>4132096</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>30273960</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>125279007</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>378149106</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>934066670</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>2008283517</v>
+      </c>
+      <c r="AE5">
+        <v>3900009866</v>
+      </c>
+      <c r="AF5">
+        <v>7006303130</v>
+      </c>
+      <c r="AG5">
+        <v>11835956777</v>
+      </c>
+      <c r="AH5">
+        <v>19023389376</v>
+      </c>
+      <c r="AI5">
+        <v>29342533340</v>
+      </c>
+      <c r="AJ5">
+        <v>43720723787</v>
+      </c>
+      <c r="AK5">
+        <v>63252587636</v>
+      </c>
+      <c r="AL5">
+        <v>89213932300</v>
+      </c>
+      <c r="AM5">
+        <v>374548765406</v>
+      </c>
+      <c r="AN5">
+        <v>2833633333350</v>
+      </c>
+      <c r="AO5">
+        <v>11918612345627</v>
+      </c>
+      <c r="AP5">
+        <v>36331925154256</v>
+      </c>
+      <c r="AQ5">
+        <v>1160013040123320</v>
+      </c>
+      <c r="AR5">
+        <v>3.7078715432098496E+16</v>
+      </c>
+      <c r="AS5">
+        <v>2.8146097708333299E+17</v>
+      </c>
+      <c r="AT5">
+        <v>1.18585194567901E+18</v>
+      </c>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>400</v>
       </c>
-      <c r="C6" s="2">
-        <v>13400</v>
-      </c>
-      <c r="D6" s="2">
-        <v>451111</v>
-      </c>
-      <c r="E6" s="2">
-        <v>9202559</v>
-      </c>
-      <c r="F6" s="2">
-        <v>126835109</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1269817428</v>
-      </c>
-      <c r="H6" s="2">
-        <v>9727994039</v>
-      </c>
-      <c r="I6" s="2">
-        <v>59323995199</v>
-      </c>
-      <c r="J6" s="2">
-        <v>297074585225</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="C6">
+        <v>13333</v>
+      </c>
+      <c r="D6" s="6">
+        <v>447778</v>
+      </c>
+      <c r="E6">
+        <v>9111650</v>
+      </c>
+      <c r="F6" s="5">
+        <v>125279007</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1251251004</v>
+      </c>
+      <c r="H6" s="6">
+        <v>9563419823</v>
+      </c>
+      <c r="I6" s="6">
+        <v>58187547820</v>
+      </c>
+      <c r="J6" s="6">
+        <v>290737409717</v>
+      </c>
+      <c r="K6" s="6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6">
         <v>3</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="6">
         <v>5</v>
       </c>
-      <c r="M6" s="3">
-        <v>7</v>
-      </c>
-      <c r="N6" s="3"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
+      <c r="N6" s="6">
+        <v>3972999029388</v>
+      </c>
+      <c r="X6">
+        <v>407254</v>
+      </c>
+      <c r="Y6">
+        <v>21591496</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>230282157</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>1251251004</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>4677232746</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>13777258407</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>34403401347</v>
+      </c>
+      <c r="AE6">
+        <v>76095935946</v>
+      </c>
+      <c r="AF6">
+        <v>153386909107</v>
+      </c>
+      <c r="AG6">
+        <v>287302124354</v>
+      </c>
+      <c r="AH6">
+        <v>507061538596</v>
+      </c>
+      <c r="AI6">
+        <v>851978071757</v>
+      </c>
+      <c r="AJ6">
+        <v>1373554828954</v>
+      </c>
+      <c r="AK6">
+        <v>2137780735339</v>
+      </c>
+      <c r="AL6">
+        <v>3227624583857</v>
+      </c>
+      <c r="AM6">
+        <v>18009528118246</v>
+      </c>
+      <c r="AN6">
+        <v>203717871698607</v>
+      </c>
+      <c r="AO6">
+        <v>1140639187958100</v>
+      </c>
+      <c r="AP6">
+        <v>4342096628285490</v>
+      </c>
+      <c r="AQ6">
+        <v>2.7673214339696E+17</v>
+      </c>
+      <c r="AR6">
+        <v>1.76737460360657E+19</v>
+      </c>
+      <c r="AS6">
+        <v>2.01174232157437E+20</v>
+      </c>
+      <c r="AT6">
+        <v>1.12993337569593E+21</v>
+      </c>
     </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>500</v>
       </c>
-      <c r="C7" s="2">
-        <v>20917</v>
-      </c>
-      <c r="D7" s="2">
-        <v>878472</v>
-      </c>
-      <c r="E7" s="2">
-        <v>22313025</v>
-      </c>
-      <c r="F7" s="2">
-        <v>381911546</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4732871282</v>
-      </c>
-      <c r="H7" s="2">
-        <v>44709647908</v>
-      </c>
-      <c r="I7" s="2">
-        <v>334740200089</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2048073072881</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="C7">
+        <v>20833</v>
+      </c>
+      <c r="D7" s="5">
+        <v>873264</v>
+      </c>
+      <c r="E7">
+        <v>22136264</v>
+      </c>
+      <c r="F7" s="5">
+        <v>378149106</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4677232746</v>
+      </c>
+      <c r="H7" s="6">
+        <v>44100541271</v>
+      </c>
+      <c r="I7" s="6">
+        <v>329567334191</v>
+      </c>
+      <c r="J7" s="6">
+        <v>2012762670309</v>
+      </c>
+      <c r="K7" s="6">
+        <v>2</v>
+      </c>
+      <c r="L7" s="6">
         <v>3</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="6">
         <v>5</v>
       </c>
-      <c r="M7" s="3">
-        <v>7</v>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
+      <c r="N7" s="6">
+        <v>230793554364681</v>
+      </c>
+      <c r="X7">
+        <v>930912</v>
+      </c>
+      <c r="Y7">
+        <v>87914929</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>1348858067</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>9563419823</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>44100541271</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>154504465228</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>447249407247</v>
+      </c>
+      <c r="AE7">
+        <v>1125143036082</v>
+      </c>
+      <c r="AF7">
+        <v>2541858922420</v>
+      </c>
+      <c r="AG7">
+        <v>5274078114658</v>
+      </c>
+      <c r="AH7">
+        <v>10213720000299</v>
+      </c>
+      <c r="AI7">
+        <v>18682742611831</v>
+      </c>
+      <c r="AJ7">
+        <v>32572992535850</v>
+      </c>
+      <c r="AK7">
+        <v>54513584583967</v>
+      </c>
+      <c r="AL7">
+        <v>88068291384398</v>
+      </c>
+      <c r="AM7">
+        <v>652203260080370</v>
+      </c>
+      <c r="AN7">
+        <v>1.10153245218577E+16</v>
+      </c>
+      <c r="AO7">
+        <v>8.2044581957463008E+16</v>
+      </c>
+      <c r="AP7">
+        <v>3.8985835339933798E+17</v>
+      </c>
+      <c r="AQ7">
+        <v>4.9554823670218498E+19</v>
+      </c>
+      <c r="AR7">
+        <v>6.3208891385988E+21</v>
+      </c>
+      <c r="AS7">
+        <v>1.07872498035519E+23</v>
+      </c>
+      <c r="AT7">
+        <v>8.0766023856325005E+23</v>
+      </c>
     </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>600</v>
       </c>
-      <c r="C8" s="2">
-        <v>30100</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1515000</v>
-      </c>
-      <c r="E8" s="2">
-        <v>46055755</v>
-      </c>
-      <c r="F8" s="2">
-        <v>941817895</v>
-      </c>
-      <c r="G8" s="2">
-        <v>13914026520</v>
-      </c>
-      <c r="H8" s="2">
-        <v>156286689060</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1387159599492</v>
-      </c>
-      <c r="J8" s="2">
-        <v>10028114108467</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="C8">
+        <v>30000</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1507500</v>
+      </c>
+      <c r="E8">
+        <v>45751225</v>
+      </c>
+      <c r="F8" s="5">
+        <v>934066670</v>
+      </c>
+      <c r="G8" s="5">
+        <v>13777258407</v>
+      </c>
+      <c r="H8" s="5">
+        <v>154504465228</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1369195210284</v>
+      </c>
+      <c r="J8" s="5">
+        <v>9883035101087</v>
+      </c>
+      <c r="K8" s="5">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5">
         <v>3</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="5">
         <v>5</v>
       </c>
-      <c r="M8" s="3">
-        <v>7</v>
-      </c>
-      <c r="N8" s="3"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
+      <c r="N8" s="5">
+        <v>9253082936723600</v>
+      </c>
+      <c r="X8">
+        <v>1786528</v>
+      </c>
+      <c r="Y8">
+        <v>290766028</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>6333941094</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>58187547820</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>329567334191</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>1369195210284</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>4584593125931</v>
+      </c>
+      <c r="AE8">
+        <v>13096052352454</v>
+      </c>
+      <c r="AF8">
+        <v>33116063658307</v>
+      </c>
+      <c r="AG8">
+        <v>76037051194142</v>
+      </c>
+      <c r="AH8">
+        <v>161437810222893</v>
+      </c>
+      <c r="AI8">
+        <v>321246606137759</v>
+      </c>
+      <c r="AJ8">
+        <v>605326449545154</v>
+      </c>
+      <c r="AK8">
+        <v>1088775619507180</v>
+      </c>
+      <c r="AL8">
+        <v>1881264064337910</v>
+      </c>
+      <c r="AM8">
+        <v>1.84611298173173E+16</v>
+      </c>
+      <c r="AN8">
+        <v>4.6478725099977901E+17</v>
+      </c>
+      <c r="AO8">
+        <v>4.60134347264691E+18</v>
+      </c>
+      <c r="AP8">
+        <v>2.7279292827788702E+19</v>
+      </c>
+      <c r="AQ8">
+        <v>6.9087707290873899E+21</v>
+      </c>
+      <c r="AR8">
+        <v>1.7591387165348501E+24</v>
+      </c>
+      <c r="AS8">
+        <v>4.50038086335053E+25</v>
+      </c>
+      <c r="AT8">
+        <v>4.4912640746291998E+26</v>
+      </c>
     </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>700</v>
       </c>
-      <c r="C9" s="2">
-        <v>40950</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2402361</v>
-      </c>
-      <c r="E9" s="2">
-        <v>85043249</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2022576869</v>
-      </c>
-      <c r="G9" s="2">
-        <v>34696437288</v>
-      </c>
-      <c r="H9" s="2">
-        <v>451678463853</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4636266938051</v>
-      </c>
-      <c r="J9" s="2">
-        <v>38667208407883</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="C9">
+        <v>40833</v>
+      </c>
+      <c r="D9">
+        <v>2392153</v>
+      </c>
+      <c r="E9">
+        <v>84560700</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2008283517</v>
+      </c>
+      <c r="G9" s="5">
+        <v>34403401347</v>
+      </c>
+      <c r="H9" s="5">
+        <v>447249407247</v>
+      </c>
+      <c r="I9" s="5">
+        <v>4584593125931</v>
+      </c>
+      <c r="J9" s="5">
+        <v>38185308620564</v>
+      </c>
+      <c r="K9" s="5">
+        <v>2</v>
+      </c>
+      <c r="L9" s="5">
         <v>3</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="5">
         <v>5</v>
       </c>
-      <c r="M9" s="3">
-        <v>7</v>
-      </c>
-      <c r="N9" s="3"/>
+      <c r="N9" s="5">
+        <v>2.7936332848370202E+17</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
@@ -889,52 +1373,116 @@
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
+      <c r="X9" s="7">
+        <v>2977866</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>807151588</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>24613920986</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>290737409717</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>2012762670309</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>9883035101087</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>38185308620564</v>
+      </c>
+      <c r="AE9">
+        <v>123626898222812</v>
+      </c>
+      <c r="AF9">
+        <v>349407773809712</v>
+      </c>
+      <c r="AG9">
+        <v>886745696653253</v>
+      </c>
+      <c r="AH9">
+        <v>2062053737498140</v>
+      </c>
+      <c r="AI9">
+        <v>4460219326165600</v>
+      </c>
+      <c r="AJ9">
+        <v>9076962366548020</v>
+      </c>
+      <c r="AK9">
+        <v>1.75360539081224E+16</v>
+      </c>
+      <c r="AL9">
+        <v>3.23902563955393E+16</v>
+      </c>
+      <c r="AM9">
+        <v>4.2040955859086298E+17</v>
+      </c>
+      <c r="AN9">
+        <v>1.5748687013194101E+19</v>
+      </c>
+      <c r="AO9">
+        <v>2.07035979156171E+20</v>
+      </c>
+      <c r="AP9">
+        <v>1.5305250421124099E+21</v>
+      </c>
+      <c r="AQ9">
+        <v>7.7144167298733097E+23</v>
+      </c>
+      <c r="AR9">
+        <v>3.9188732492306802E+26</v>
+      </c>
+      <c r="AS9">
+        <v>1.5026023070381199E+28</v>
+      </c>
+      <c r="AT9">
+        <v>1.9985876689037601E+29</v>
+      </c>
     </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>800</v>
       </c>
-      <c r="C10" s="2">
-        <v>53467</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3582222</v>
-      </c>
-      <c r="E10" s="2">
-        <v>144721340</v>
-      </c>
-      <c r="F10" s="2">
-        <v>3924308381</v>
-      </c>
-      <c r="G10" s="2">
-        <v>76663512392</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1134904074747</v>
-      </c>
-      <c r="I10" s="2">
-        <v>13225427691101</v>
-      </c>
-      <c r="J10" s="2">
-        <v>124995134376940</v>
-      </c>
-      <c r="K10" s="3">
+      <c r="C10">
+        <v>53333</v>
+      </c>
+      <c r="D10">
+        <v>3568889</v>
+      </c>
+      <c r="E10">
+        <v>144002189</v>
+      </c>
+      <c r="F10">
+        <v>3900009866</v>
+      </c>
+      <c r="G10">
+        <v>76095935946</v>
+      </c>
+      <c r="H10">
+        <v>1125143036082</v>
+      </c>
+      <c r="I10">
+        <v>13096052352454</v>
+      </c>
+      <c r="J10">
+        <v>123626898222812</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
         <v>3</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10">
         <v>5</v>
       </c>
-      <c r="M10" s="3">
-        <v>7</v>
-      </c>
-      <c r="N10" s="3"/>
+      <c r="N10">
+        <v>6.7270900517410396E+18</v>
+      </c>
       <c r="O10" s="7"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -944,52 +1492,116 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
+      <c r="X10" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE10">
+        <v>2</v>
+      </c>
+      <c r="AF10">
+        <v>2</v>
+      </c>
+      <c r="AG10">
+        <v>2</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AI10">
+        <v>2</v>
+      </c>
+      <c r="AJ10">
+        <v>2</v>
+      </c>
+      <c r="AK10">
+        <v>2</v>
+      </c>
+      <c r="AL10">
+        <v>2</v>
+      </c>
+      <c r="AM10">
+        <v>2</v>
+      </c>
+      <c r="AN10">
+        <v>2</v>
+      </c>
+      <c r="AO10">
+        <v>2</v>
+      </c>
+      <c r="AP10">
+        <v>2</v>
+      </c>
+      <c r="AQ10">
+        <v>2</v>
+      </c>
+      <c r="AR10">
+        <v>2</v>
+      </c>
+      <c r="AS10">
+        <v>2</v>
+      </c>
+      <c r="AT10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>900</v>
       </c>
-      <c r="C11" s="3">
-        <v>67650</v>
-      </c>
-      <c r="D11" s="3">
-        <v>5096250</v>
-      </c>
-      <c r="E11" s="3">
-        <v>231369195</v>
-      </c>
-      <c r="F11" s="3">
-        <v>7045118405</v>
-      </c>
-      <c r="G11" s="3">
-        <v>154404470830</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2561478643574</v>
-      </c>
-      <c r="I11" s="3">
-        <v>33407250281517</v>
-      </c>
-      <c r="J11" s="3">
-        <v>352851241223889</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="C11">
+        <v>67500</v>
+      </c>
+      <c r="D11">
+        <v>5079375</v>
+      </c>
+      <c r="E11">
+        <v>230346525</v>
+      </c>
+      <c r="F11">
+        <v>7006303130</v>
+      </c>
+      <c r="G11">
+        <v>153386909107</v>
+      </c>
+      <c r="H11">
+        <v>2541858922420</v>
+      </c>
+      <c r="I11">
+        <v>33116063658307</v>
+      </c>
+      <c r="J11">
+        <v>349407773809712</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
         <v>3</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11">
         <v>5</v>
       </c>
-      <c r="M11" s="3">
-        <v>7</v>
-      </c>
-      <c r="N11" s="3"/>
+      <c r="N11">
+        <v>1.34508188001572E+20</v>
+      </c>
       <c r="O11" s="7"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -999,52 +1611,116 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
+      <c r="X11" s="6">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+      <c r="AF11">
+        <v>3</v>
+      </c>
+      <c r="AG11">
+        <v>3</v>
+      </c>
+      <c r="AH11">
+        <v>3</v>
+      </c>
+      <c r="AI11">
+        <v>3</v>
+      </c>
+      <c r="AJ11">
+        <v>3</v>
+      </c>
+      <c r="AK11">
+        <v>3</v>
+      </c>
+      <c r="AL11">
+        <v>3</v>
+      </c>
+      <c r="AM11">
+        <v>3</v>
+      </c>
+      <c r="AN11">
+        <v>3</v>
+      </c>
+      <c r="AO11">
+        <v>3</v>
+      </c>
+      <c r="AP11">
+        <v>3</v>
+      </c>
+      <c r="AQ11">
+        <v>3</v>
+      </c>
+      <c r="AR11">
+        <v>3</v>
+      </c>
+      <c r="AS11">
+        <v>3</v>
+      </c>
+      <c r="AT11">
+        <v>3</v>
+      </c>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12" s="3">
-        <v>83500</v>
-      </c>
-      <c r="D12" s="3">
-        <v>6986111</v>
-      </c>
-      <c r="E12" s="3">
-        <v>352099314</v>
-      </c>
-      <c r="F12" s="3">
-        <v>11894988004</v>
-      </c>
-      <c r="G12" s="3">
-        <v>289018309991</v>
-      </c>
-      <c r="H12" s="3">
-        <v>5310743503299</v>
-      </c>
-      <c r="I12" s="3">
-        <v>76639419601247</v>
-      </c>
-      <c r="J12" s="3">
-        <v>894622011523232</v>
-      </c>
-      <c r="K12" s="3">
+      <c r="C12">
+        <v>83333</v>
+      </c>
+      <c r="D12">
+        <v>6965278</v>
+      </c>
+      <c r="E12">
+        <v>350697875</v>
+      </c>
+      <c r="F12">
+        <v>11835956777</v>
+      </c>
+      <c r="G12">
+        <v>287302124354</v>
+      </c>
+      <c r="H12">
+        <v>5274078114658</v>
+      </c>
+      <c r="I12">
+        <v>76037051194142</v>
+      </c>
+      <c r="J12">
+        <v>886745696653253</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
         <v>3</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12">
         <v>5</v>
       </c>
-      <c r="M12" s="3">
-        <v>7</v>
-      </c>
-      <c r="N12" s="3"/>
+      <c r="N12">
+        <v>2.3001650325743201E+21</v>
+      </c>
       <c r="O12" s="7"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1054,52 +1730,116 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
+      <c r="X12" s="6">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE12">
+        <v>5</v>
+      </c>
+      <c r="AF12">
+        <v>5</v>
+      </c>
+      <c r="AG12">
+        <v>5</v>
+      </c>
+      <c r="AH12">
+        <v>5</v>
+      </c>
+      <c r="AI12">
+        <v>5</v>
+      </c>
+      <c r="AJ12">
+        <v>5</v>
+      </c>
+      <c r="AK12">
+        <v>5</v>
+      </c>
+      <c r="AL12">
+        <v>5</v>
+      </c>
+      <c r="AM12">
+        <v>5</v>
+      </c>
+      <c r="AN12">
+        <v>5</v>
+      </c>
+      <c r="AO12">
+        <v>5</v>
+      </c>
+      <c r="AP12">
+        <v>5</v>
+      </c>
+      <c r="AQ12">
+        <v>5</v>
+      </c>
+      <c r="AR12">
+        <v>5</v>
+      </c>
+      <c r="AS12">
+        <v>5</v>
+      </c>
+      <c r="AT12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>1100</v>
       </c>
-      <c r="C13" s="3">
-        <v>101017</v>
-      </c>
-      <c r="D13" s="3">
-        <v>9293472</v>
-      </c>
-      <c r="E13" s="3">
-        <v>514857530</v>
-      </c>
-      <c r="F13" s="3">
-        <v>19109662091</v>
-      </c>
-      <c r="G13" s="3">
-        <v>509816186702</v>
-      </c>
-      <c r="H13" s="3">
-        <v>10278310477111</v>
-      </c>
-      <c r="I13" s="3">
-        <v>162601477536085</v>
-      </c>
-      <c r="J13" s="3">
-        <v>2078723886265530</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="C13">
+        <v>100833</v>
+      </c>
+      <c r="D13">
+        <v>9268264</v>
+      </c>
+      <c r="E13">
+        <v>512993739</v>
+      </c>
+      <c r="F13">
+        <v>19023389376</v>
+      </c>
+      <c r="G13">
+        <v>507061538596</v>
+      </c>
+      <c r="H13">
+        <v>10213720000299</v>
+      </c>
+      <c r="I13">
+        <v>161437810222893</v>
+      </c>
+      <c r="J13">
+        <v>2062053737498140</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
         <v>3</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13">
         <v>5</v>
       </c>
-      <c r="M13" s="3">
-        <v>7</v>
-      </c>
-      <c r="N13" s="3"/>
+      <c r="N13">
+        <v>3.4403115367205001E+22</v>
+      </c>
       <c r="O13" s="7"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -1109,52 +1849,107 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
+      <c r="X13" s="6">
+        <v>204226</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>190569292</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>40853235313</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>3972999029388</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>230793554364681</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>9253082936723600</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>2.7936332848370202E+17</v>
+      </c>
+      <c r="AE13">
+        <v>6.7270900517410396E+18</v>
+      </c>
+      <c r="AF13">
+        <v>1.34508188001572E+20</v>
+      </c>
+      <c r="AG13">
+        <v>2.3001650325743201E+21</v>
+      </c>
+      <c r="AH13">
+        <v>3.4403115367205001E+22</v>
+      </c>
+      <c r="AI13">
+        <v>4.5800478800814402E+23</v>
+      </c>
+      <c r="AJ13">
+        <v>5.5036377624997203E+24</v>
+      </c>
+      <c r="AK13">
+        <v>6.0378285202834401E+25</v>
+      </c>
+      <c r="AL13">
+        <v>6.1045074711796603E+26</v>
+      </c>
+      <c r="AM13">
+        <v>2.4061467864032602E+31</v>
+      </c>
+      <c r="AN13">
+        <v>1.32946169076319E+39</v>
+      </c>
+      <c r="AO13">
+        <v>4.72081917561941E+45</v>
+      </c>
+      <c r="AP13">
+        <v>2.8708755106413501E+51</v>
+      </c>
+      <c r="AQ13">
+        <v>1.6982016882544199E+74</v>
+      </c>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1200</v>
       </c>
-      <c r="C14" s="3">
-        <v>120200</v>
-      </c>
-      <c r="D14" s="3">
-        <v>12060000</v>
-      </c>
-      <c r="E14" s="3">
-        <v>728423010</v>
-      </c>
-      <c r="F14" s="3">
-        <v>29464538290</v>
-      </c>
-      <c r="G14" s="3">
-        <v>856222210840</v>
-      </c>
-      <c r="H14" s="3">
-        <v>18791100403613</v>
-      </c>
-      <c r="I14" s="3">
-        <v>323370783523261</v>
-      </c>
-      <c r="J14" s="3">
-        <v>4493304421998500</v>
-      </c>
-      <c r="K14" s="3">
+      <c r="C14">
+        <v>120000</v>
+      </c>
+      <c r="D14">
+        <v>12030000</v>
+      </c>
+      <c r="E14">
+        <v>726004950</v>
+      </c>
+      <c r="F14">
+        <v>29342533340</v>
+      </c>
+      <c r="G14">
+        <v>851978071757</v>
+      </c>
+      <c r="H14">
+        <v>18682742611831</v>
+      </c>
+      <c r="I14">
+        <v>321246606137759</v>
+      </c>
+      <c r="J14">
+        <v>4460219326165600</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
         <v>3</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14">
         <v>5</v>
       </c>
-      <c r="M14" s="3">
-        <v>7</v>
-      </c>
-      <c r="N14" s="3"/>
+      <c r="N14">
+        <v>4.5800478800814402E+23</v>
+      </c>
       <c r="O14" s="7"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -1172,44 +1967,46 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1300</v>
       </c>
-      <c r="C15" s="3">
-        <v>141050</v>
-      </c>
-      <c r="D15" s="3">
-        <v>15327361</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1002408254</v>
-      </c>
-      <c r="F15" s="3">
-        <v>43888556014</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1379872651608</v>
-      </c>
-      <c r="H15" s="3">
-        <v>32747456066663</v>
-      </c>
-      <c r="I15" s="3">
-        <v>609023445489943</v>
-      </c>
-      <c r="J15" s="3">
-        <v>9139165989440510</v>
-      </c>
-      <c r="K15" s="3">
+      <c r="C15">
+        <v>140833</v>
+      </c>
+      <c r="D15">
+        <v>15292153</v>
+      </c>
+      <c r="E15">
+        <v>999335675</v>
+      </c>
+      <c r="F15">
+        <v>43720723787</v>
+      </c>
+      <c r="G15">
+        <v>1373554828954</v>
+      </c>
+      <c r="H15">
+        <v>32572992535850</v>
+      </c>
+      <c r="I15">
+        <v>605326449545154</v>
+      </c>
+      <c r="J15">
+        <v>9076962366548020</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
         <v>3</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15">
         <v>5</v>
       </c>
-      <c r="M15" s="3">
-        <v>7</v>
-      </c>
-      <c r="N15" s="3"/>
+      <c r="N15">
+        <v>5.5036377624997203E+24</v>
+      </c>
       <c r="O15" s="7"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -1225,44 +2022,46 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1400</v>
       </c>
-      <c r="C16" s="3">
-        <v>163567</v>
-      </c>
-      <c r="D16" s="3">
-        <v>19137222</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1347259095</v>
-      </c>
-      <c r="F16" s="3">
-        <v>63478085176</v>
-      </c>
-      <c r="G16" s="8">
-        <v>2146913556712</v>
-      </c>
-      <c r="H16" s="8">
-        <v>54784809688750</v>
-      </c>
-      <c r="I16" s="8">
-        <v>1094953568823150</v>
-      </c>
-      <c r="J16" s="8">
-        <v>1.7647722935916E+16</v>
-      </c>
-      <c r="K16" s="8">
+      <c r="C16">
+        <v>163333</v>
+      </c>
+      <c r="D16">
+        <v>19096389</v>
+      </c>
+      <c r="E16">
+        <v>1343423414</v>
+      </c>
+      <c r="F16">
+        <v>63252587636</v>
+      </c>
+      <c r="G16">
+        <v>2137780735339</v>
+      </c>
+      <c r="H16">
+        <v>54513584583967</v>
+      </c>
+      <c r="I16">
+        <v>1088775619507180</v>
+      </c>
+      <c r="J16">
+        <v>1.75360539081224E+16</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
         <v>3</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16">
         <v>5</v>
       </c>
-      <c r="M16" s="8">
-        <v>7</v>
-      </c>
-      <c r="N16" s="3"/>
+      <c r="N16">
+        <v>6.0378285202834401E+25</v>
+      </c>
       <c r="O16" s="7"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -1282,40 +2081,42 @@
       <c r="B17" s="1">
         <v>1500</v>
       </c>
-      <c r="C17" s="3">
-        <v>187750</v>
-      </c>
-      <c r="D17" s="3">
-        <v>23531250</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1774254700</v>
-      </c>
-      <c r="F17" s="3">
-        <v>89510815050</v>
-      </c>
-      <c r="G17" s="8">
-        <v>3240496784050</v>
-      </c>
-      <c r="H17" s="8">
-        <v>88477385146677</v>
-      </c>
-      <c r="I17" s="8">
-        <v>1891231728363360</v>
-      </c>
-      <c r="J17" s="8">
-        <v>3.25828854201028E+16</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="C17">
+        <v>187500</v>
+      </c>
+      <c r="D17">
+        <v>23484375</v>
+      </c>
+      <c r="E17">
+        <v>1769539000</v>
+      </c>
+      <c r="F17">
+        <v>89213932300</v>
+      </c>
+      <c r="G17">
+        <v>3227624583857</v>
+      </c>
+      <c r="H17">
+        <v>88068291384398</v>
+      </c>
+      <c r="I17">
+        <v>1881264064337910</v>
+      </c>
+      <c r="J17">
+        <v>3.23902563955393E+16</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
         <v>3</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17">
         <v>5</v>
       </c>
-      <c r="M17" s="8">
-        <v>7</v>
-      </c>
-      <c r="N17" s="3"/>
+      <c r="N17">
+        <v>6.1045074711796603E+26</v>
+      </c>
       <c r="O17" s="7"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
@@ -1345,40 +2146,42 @@
       <c r="B18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18" s="3">
-        <v>333667</v>
-      </c>
-      <c r="D18" s="3">
-        <v>55722222</v>
-      </c>
-      <c r="E18" s="3">
-        <v>5594508350</v>
-      </c>
-      <c r="F18" s="3">
-        <v>375483964471</v>
-      </c>
-      <c r="G18" s="8">
-        <v>18063436158832</v>
-      </c>
-      <c r="H18" s="8">
-        <v>654478064673960</v>
-      </c>
-      <c r="I18" s="8">
-        <v>1.85346098736255E+16</v>
-      </c>
-      <c r="J18" s="8">
-        <v>4.2228883290359802E+17</v>
-      </c>
-      <c r="K18" s="8">
+      <c r="C18">
+        <v>333333</v>
+      </c>
+      <c r="D18">
+        <v>55638889</v>
+      </c>
+      <c r="E18">
+        <v>5583347139</v>
+      </c>
+      <c r="F18">
+        <v>374548765406</v>
+      </c>
+      <c r="G18">
+        <v>18009528118246</v>
+      </c>
+      <c r="H18">
+        <v>652203260080370</v>
+      </c>
+      <c r="I18">
+        <v>1.84611298173173E+16</v>
+      </c>
+      <c r="J18">
+        <v>4.2040955859086298E+17</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
         <v>3</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18">
         <v>5</v>
       </c>
-      <c r="M18" s="8">
-        <v>7</v>
-      </c>
-      <c r="N18" s="3"/>
+      <c r="N18">
+        <v>2.4061467864032602E+31</v>
+      </c>
       <c r="O18" s="7"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
@@ -1408,40 +2211,42 @@
       <c r="B19" s="1">
         <v>3000</v>
       </c>
-      <c r="C19" s="3">
-        <v>750500</v>
-      </c>
-      <c r="D19" s="3">
-        <v>187875000</v>
-      </c>
-      <c r="E19" s="3">
-        <v>28256393775</v>
-      </c>
-      <c r="F19" s="3">
-        <v>2838352114475</v>
-      </c>
-      <c r="G19" s="8">
-        <v>204124699710600</v>
-      </c>
-      <c r="H19" s="8">
-        <v>1.10409673891502E+16</v>
-      </c>
-      <c r="I19" s="8">
-        <v>4.6602258787669702E+17</v>
-      </c>
-      <c r="J19" s="8">
-        <v>1.5795722712310901E+19</v>
-      </c>
-      <c r="K19" s="8">
+      <c r="C19">
+        <v>750000</v>
+      </c>
+      <c r="D19">
+        <v>187687500</v>
+      </c>
+      <c r="E19">
+        <v>28218781125</v>
+      </c>
+      <c r="F19">
+        <v>2833633333350</v>
+      </c>
+      <c r="G19">
+        <v>203717871698607</v>
+      </c>
+      <c r="H19">
+        <v>1.10153245218577E+16</v>
+      </c>
+      <c r="I19">
+        <v>4.6478725099977901E+17</v>
+      </c>
+      <c r="J19">
+        <v>1.5748687013194101E+19</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
         <v>3</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19">
         <v>5</v>
       </c>
-      <c r="M19" s="8">
-        <v>7</v>
-      </c>
-      <c r="N19" s="3"/>
+      <c r="N19">
+        <v>1.32946169076319E+39</v>
+      </c>
       <c r="O19" s="7"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -1471,40 +2276,42 @@
       <c r="B20" s="1">
         <v>4000</v>
       </c>
-      <c r="C20" s="3">
-        <v>1334000</v>
-      </c>
-      <c r="D20" s="3">
-        <v>445111111</v>
-      </c>
-      <c r="E20" s="3">
-        <v>89200255589</v>
-      </c>
-      <c r="F20" s="3">
-        <v>11933501289979</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1142348229996940</v>
-      </c>
-      <c r="H20" s="8">
-        <v>8.2187910023853408E+16</v>
-      </c>
-      <c r="I20" s="8">
-        <v>4.6105233020709202E+18</v>
-      </c>
-      <c r="J20" s="8">
-        <v>2.0750025041541399E+20</v>
-      </c>
-      <c r="K20" s="8">
+      <c r="C20">
+        <v>1333333</v>
+      </c>
+      <c r="D20">
+        <v>444777778</v>
+      </c>
+      <c r="E20">
+        <v>89111166500</v>
+      </c>
+      <c r="F20">
+        <v>11918612345627</v>
+      </c>
+      <c r="G20">
+        <v>1140639187958100</v>
+      </c>
+      <c r="H20">
+        <v>8.2044581957463008E+16</v>
+      </c>
+      <c r="I20">
+        <v>4.60134347264691E+18</v>
+      </c>
+      <c r="J20">
+        <v>2.07035979156171E+20</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
         <v>3</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20">
         <v>5</v>
       </c>
-      <c r="M20" s="8">
-        <v>7</v>
-      </c>
-      <c r="N20" s="3"/>
+      <c r="N20">
+        <v>4.72081917561941E+45</v>
+      </c>
       <c r="O20" s="7"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -1534,40 +2341,42 @@
       <c r="B21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21" s="3">
-        <v>2084167</v>
-      </c>
-      <c r="D21" s="3">
-        <v>869097222</v>
-      </c>
-      <c r="E21" s="3">
-        <v>217621927125</v>
-      </c>
-      <c r="F21" s="3">
-        <v>36368238898446</v>
-      </c>
-      <c r="G21" s="8">
-        <v>4347302470536430</v>
-      </c>
-      <c r="H21" s="8">
-        <v>3.9040339416227802E+17</v>
-      </c>
-      <c r="I21" s="8">
-        <v>2.7322852856004698E+19</v>
-      </c>
-      <c r="J21" s="8">
-        <v>1.533272596169E+21</v>
-      </c>
-      <c r="K21" s="8">
+      <c r="C21">
+        <v>2083333</v>
+      </c>
+      <c r="D21">
+        <v>868576389</v>
+      </c>
+      <c r="E21">
+        <v>217448003264</v>
+      </c>
+      <c r="F21">
+        <v>36331925154256</v>
+      </c>
+      <c r="G21">
+        <v>4342096628285490</v>
+      </c>
+      <c r="H21">
+        <v>3.8985835339933798E+17</v>
+      </c>
+      <c r="I21">
+        <v>2.7279292827788702E+19</v>
+      </c>
+      <c r="J21">
+        <v>1.5305250421124099E+21</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
         <v>3</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21">
         <v>5</v>
       </c>
-      <c r="M21" s="8">
-        <v>7</v>
-      </c>
-      <c r="N21" s="3"/>
+      <c r="N21">
+        <v>2.8708755106413501E+51</v>
+      </c>
       <c r="O21" s="7"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -1597,40 +2406,42 @@
       <c r="B22" s="1">
         <v>10000</v>
       </c>
-      <c r="C22" s="3">
-        <v>8335000</v>
-      </c>
-      <c r="D22" s="3">
-        <v>6948611111</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3477084930639</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1160592901581420</v>
-      </c>
-      <c r="G22" s="8">
-        <v>2.7689810809092E+17</v>
-      </c>
-      <c r="H22" s="8">
-        <v>4.9589487815766499E+19</v>
-      </c>
-      <c r="I22" s="8">
-        <v>6.9142922330439303E+21</v>
-      </c>
-      <c r="J22" s="8">
-        <v>7.7213503618299507E+23</v>
-      </c>
-      <c r="K22" s="8">
+      <c r="C22">
+        <v>8333333</v>
+      </c>
+      <c r="D22">
+        <v>6946527778</v>
+      </c>
+      <c r="E22">
+        <v>3475694791250</v>
+      </c>
+      <c r="F22">
+        <v>1160013040123320</v>
+      </c>
+      <c r="G22">
+        <v>2.7673214339696E+17</v>
+      </c>
+      <c r="H22">
+        <v>4.9554823670218498E+19</v>
+      </c>
+      <c r="I22">
+        <v>6.9087707290873899E+21</v>
+      </c>
+      <c r="J22">
+        <v>7.7144167298733097E+23</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
         <v>3</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22">
         <v>5</v>
       </c>
-      <c r="M22" s="8">
-        <v>7</v>
-      </c>
-      <c r="N22" s="3"/>
+      <c r="N22">
+        <v>1.6982016882544199E+74</v>
+      </c>
       <c r="O22" s="7"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -1660,40 +2471,39 @@
       <c r="B23" s="1">
         <v>20000</v>
       </c>
-      <c r="C23" s="3">
-        <v>33336667</v>
-      </c>
-      <c r="D23" s="3">
-        <v>55572222222</v>
-      </c>
-      <c r="E23" s="3">
-        <v>55594450833500</v>
-      </c>
-      <c r="F23" s="3">
-        <v>3.70879839520058E+16</v>
-      </c>
-      <c r="G23" s="8">
-        <v>1.7679046967901499E+19</v>
-      </c>
-      <c r="H23" s="8">
-        <v>6.3231006763002196E+21</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1.7598420206522899E+24</v>
-      </c>
-      <c r="J23" s="8">
-        <v>3.9206355537377398E+26</v>
-      </c>
-      <c r="K23" s="8">
+      <c r="C23">
+        <v>33333333</v>
+      </c>
+      <c r="D23">
+        <v>55563888889</v>
+      </c>
+      <c r="E23">
+        <v>55583334721389</v>
+      </c>
+      <c r="F23">
+        <v>3.7078715432098496E+16</v>
+      </c>
+      <c r="G23">
+        <v>1.76737460360657E+19</v>
+      </c>
+      <c r="H23">
+        <v>6.3208891385988E+21</v>
+      </c>
+      <c r="I23">
+        <v>1.7591387165348501E+24</v>
+      </c>
+      <c r="J23">
+        <v>3.9188732492306802E+26</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
         <v>3</v>
       </c>
-      <c r="L23" s="8">
+      <c r="M23">
         <v>5</v>
       </c>
-      <c r="M23" s="8">
-        <v>7</v>
-      </c>
-      <c r="N23" s="3"/>
       <c r="O23" s="7"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
@@ -1723,40 +2533,39 @@
       <c r="B24" s="1">
         <v>30000</v>
       </c>
-      <c r="C24" s="3">
-        <v>75005000</v>
-      </c>
-      <c r="D24" s="3">
-        <v>187537500000</v>
-      </c>
-      <c r="E24" s="3">
-        <v>281381264375250</v>
-      </c>
-      <c r="F24" s="3">
-        <v>2.8150788333645699E+17</v>
-      </c>
-      <c r="G24" s="8">
-        <v>2.01214460972024E+20</v>
-      </c>
-      <c r="H24" s="8">
-        <v>1.07897662416109E+23</v>
-      </c>
-      <c r="I24" s="8">
-        <v>4.5015805652279704E+25</v>
-      </c>
-      <c r="J24" s="8">
-        <v>1.50305288509519E+28</v>
-      </c>
-      <c r="K24" s="8">
+      <c r="C24">
+        <v>75000000</v>
+      </c>
+      <c r="D24">
+        <v>187518750000</v>
+      </c>
+      <c r="E24">
+        <v>281343753123750</v>
+      </c>
+      <c r="F24">
+        <v>2.8146097708333299E+17</v>
+      </c>
+      <c r="G24">
+        <v>2.01174232157437E+20</v>
+      </c>
+      <c r="H24">
+        <v>1.07872498035519E+23</v>
+      </c>
+      <c r="I24">
+        <v>4.50038086335053E+25</v>
+      </c>
+      <c r="J24">
+        <v>1.5026023070381199E+28</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
         <v>3</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24">
         <v>5</v>
       </c>
-      <c r="M24" s="8">
-        <v>7</v>
-      </c>
-      <c r="N24" s="3"/>
       <c r="O24" s="7"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -1786,40 +2595,39 @@
       <c r="B25" s="1">
         <v>40000</v>
       </c>
-      <c r="C25" s="3">
-        <v>133340000</v>
-      </c>
-      <c r="D25" s="3">
-        <v>444511111111</v>
-      </c>
-      <c r="E25" s="3">
-        <v>889200025555889</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1.1860001679067799E+18</v>
-      </c>
-      <c r="G25" s="8">
-        <v>1.13010284664268E+21</v>
-      </c>
-      <c r="H25" s="8">
-        <v>8.0780155438337898E+23</v>
-      </c>
-      <c r="I25" s="8">
-        <v>4.4921621030273502E+26</v>
-      </c>
-      <c r="J25" s="8">
-        <v>1.9990371994829001E+29</v>
-      </c>
-      <c r="K25" s="8">
+      <c r="C25">
+        <v>133333333</v>
+      </c>
+      <c r="D25">
+        <v>444477777778</v>
+      </c>
+      <c r="E25">
+        <v>889111116665000</v>
+      </c>
+      <c r="F25">
+        <v>1.18585194567901E+18</v>
+      </c>
+      <c r="G25">
+        <v>1.12993337569593E+21</v>
+      </c>
+      <c r="H25">
+        <v>8.0766023856325005E+23</v>
+      </c>
+      <c r="I25">
+        <v>4.4912640746291998E+26</v>
+      </c>
+      <c r="J25">
+        <v>1.9985876689037601E+29</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
         <v>3</v>
       </c>
-      <c r="L25" s="8">
+      <c r="M25">
         <v>5</v>
       </c>
-      <c r="M25" s="8">
-        <v>7</v>
-      </c>
-      <c r="N25" s="3"/>
       <c r="O25" s="7"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
@@ -4702,7 +5510,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:A55 AT2:XFD55 B27:AS55 A56:XFD1048576 B2:N2 S14:AB14 B3:B25 Q14:Q15 N14:N25 Y23:AB25 Q17:Q25 R15:X25 C3 K11:M14 E3:M3 C4:M10">
+  <conditionalFormatting sqref="A1:XFD1 A2:A55 AT2:XFD55 B27:AS55 A56:XFD1048576 B2:N2 S14:AB14 B3:B25 Q14:Q15 Y23:AB25 Q17:Q25 R15:X25 C25:N25">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed the counting script for integers again x2.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E631A084-D210-461A-87B8-15CCDAA21DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDAD770-3417-4A15-A0CD-CE42BCAF0CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -153,6 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
-  <dimension ref="B2:AT50"/>
+  <dimension ref="B2:AP50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +547,7 @@
     <col min="42" max="42" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -586,114 +587,45 @@
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X2">
-        <v>833</v>
-      </c>
-      <c r="Y2">
-        <v>3333</v>
-      </c>
-      <c r="Z2">
-        <v>7500</v>
-      </c>
-      <c r="AA2">
-        <v>13333</v>
-      </c>
-      <c r="AB2">
-        <v>20833</v>
-      </c>
-      <c r="AC2">
-        <v>30000</v>
-      </c>
-      <c r="AD2">
-        <v>40833</v>
-      </c>
-      <c r="AE2">
-        <v>53333</v>
-      </c>
-      <c r="AF2">
-        <v>67500</v>
-      </c>
-      <c r="AG2">
-        <v>83333</v>
-      </c>
-      <c r="AH2">
-        <v>100833</v>
-      </c>
-      <c r="AI2">
-        <v>120000</v>
-      </c>
-      <c r="AJ2">
-        <v>140833</v>
-      </c>
-      <c r="AK2">
-        <v>163333</v>
-      </c>
-      <c r="AL2">
-        <v>187500</v>
-      </c>
-      <c r="AM2">
-        <v>333333</v>
-      </c>
-      <c r="AN2">
-        <v>750000</v>
-      </c>
-      <c r="AO2">
-        <v>1333333</v>
-      </c>
-      <c r="AP2">
-        <v>2083333</v>
-      </c>
-      <c r="AQ2">
-        <v>8333333</v>
-      </c>
-      <c r="AR2">
-        <v>33333333</v>
-      </c>
-      <c r="AS2">
-        <v>75000000</v>
-      </c>
-      <c r="AT2">
-        <v>133333333</v>
-      </c>
-    </row>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>833</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="8">
         <v>7153</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>38225</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>143247</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>407254</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>930912</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>1786528</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="8">
         <v>2977866</v>
       </c>
-      <c r="K3" s="6">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6">
+      <c r="K3" s="8">
+        <v>2</v>
+      </c>
+      <c r="L3" s="8">
         <v>3</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="8">
         <v>5</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="8">
         <v>204226</v>
       </c>
       <c r="P3" s="7"/>
@@ -704,664 +636,276 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
-      <c r="X3" s="7">
-        <v>7153</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>56389</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>189375</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>447778</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>873264</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>1507500</v>
-      </c>
-      <c r="AD3">
-        <v>2392153</v>
-      </c>
-      <c r="AE3">
-        <v>3568889</v>
-      </c>
-      <c r="AF3">
-        <v>5079375</v>
-      </c>
-      <c r="AG3">
-        <v>6965278</v>
-      </c>
-      <c r="AH3">
-        <v>9268264</v>
-      </c>
-      <c r="AI3">
-        <v>12030000</v>
-      </c>
-      <c r="AJ3">
-        <v>15292153</v>
-      </c>
-      <c r="AK3">
-        <v>19096389</v>
-      </c>
-      <c r="AL3">
-        <v>23484375</v>
-      </c>
-      <c r="AM3">
-        <v>55638889</v>
-      </c>
-      <c r="AN3">
-        <v>187687500</v>
-      </c>
-      <c r="AO3">
-        <v>444777778</v>
-      </c>
-      <c r="AP3">
-        <v>868576389</v>
-      </c>
-      <c r="AQ3">
-        <v>6946527778</v>
-      </c>
-      <c r="AR3">
-        <v>55563888889</v>
-      </c>
-      <c r="AS3">
-        <v>187518750000</v>
-      </c>
-      <c r="AT3">
-        <v>444477777778</v>
-      </c>
-    </row>
-    <row r="4" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X3" s="7"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>200</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>3333</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="8">
         <v>56389</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>583464</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>4132096</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>21591496</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>87914929</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>290766028</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="8">
         <v>807151588</v>
       </c>
-      <c r="K4" s="6">
-        <v>2</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="K4" s="8">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8">
         <v>3</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="8">
         <v>5</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="8">
         <v>190569292</v>
       </c>
-      <c r="X4">
-        <v>38225</v>
-      </c>
-      <c r="Y4">
-        <v>583464</v>
-      </c>
-      <c r="Z4">
-        <v>2906550</v>
-      </c>
-      <c r="AA4">
-        <v>9111650</v>
-      </c>
-      <c r="AB4">
-        <v>22136264</v>
-      </c>
-      <c r="AC4">
-        <v>45751225</v>
-      </c>
-      <c r="AD4">
-        <v>84560700</v>
-      </c>
-      <c r="AE4">
-        <v>144002189</v>
-      </c>
-      <c r="AF4">
-        <v>230346525</v>
-      </c>
-      <c r="AG4">
-        <v>350697875</v>
-      </c>
-      <c r="AH4">
-        <v>512993739</v>
-      </c>
-      <c r="AI4">
-        <v>726004950</v>
-      </c>
-      <c r="AJ4">
-        <v>999335675</v>
-      </c>
-      <c r="AK4">
-        <v>1343423414</v>
-      </c>
-      <c r="AL4">
-        <v>1769539000</v>
-      </c>
-      <c r="AM4">
-        <v>5583347139</v>
-      </c>
-      <c r="AN4">
-        <v>28218781125</v>
-      </c>
-      <c r="AO4">
-        <v>89111166500</v>
-      </c>
-      <c r="AP4">
-        <v>217448003264</v>
-      </c>
-      <c r="AQ4">
-        <v>3475694791250</v>
-      </c>
-      <c r="AR4">
-        <v>55583334721389</v>
-      </c>
-      <c r="AS4">
-        <v>281343753123750</v>
-      </c>
-      <c r="AT4">
-        <v>889111116665000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>300</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>7500</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="8">
         <v>189375</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>2906550</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>30273960</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>230282157</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="8">
         <v>1348858067</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="8">
         <v>6333941094</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="8">
         <v>24613920986</v>
       </c>
-      <c r="K5" s="6">
-        <v>2</v>
-      </c>
-      <c r="L5" s="6">
+      <c r="K5" s="8">
+        <v>2</v>
+      </c>
+      <c r="L5" s="8">
         <v>3</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="8">
         <v>5</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="8">
         <v>40853235313</v>
       </c>
-      <c r="X5">
-        <v>143247</v>
-      </c>
-      <c r="Y5">
-        <v>4132096</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>30273960</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>125279007</v>
-      </c>
-      <c r="AB5" s="5">
-        <v>378149106</v>
-      </c>
-      <c r="AC5" s="5">
-        <v>934066670</v>
-      </c>
-      <c r="AD5" s="5">
-        <v>2008283517</v>
-      </c>
-      <c r="AE5">
-        <v>3900009866</v>
-      </c>
-      <c r="AF5">
-        <v>7006303130</v>
-      </c>
-      <c r="AG5">
-        <v>11835956777</v>
-      </c>
-      <c r="AH5">
-        <v>19023389376</v>
-      </c>
-      <c r="AI5">
-        <v>29342533340</v>
-      </c>
-      <c r="AJ5">
-        <v>43720723787</v>
-      </c>
-      <c r="AK5">
-        <v>63252587636</v>
-      </c>
-      <c r="AL5">
-        <v>89213932300</v>
-      </c>
-      <c r="AM5">
-        <v>374548765406</v>
-      </c>
-      <c r="AN5">
-        <v>2833633333350</v>
-      </c>
-      <c r="AO5">
-        <v>11918612345627</v>
-      </c>
-      <c r="AP5">
-        <v>36331925154256</v>
-      </c>
-      <c r="AQ5">
-        <v>1160013040123320</v>
-      </c>
-      <c r="AR5">
-        <v>3.7078715432098496E+16</v>
-      </c>
-      <c r="AS5">
-        <v>2.8146097708333299E+17</v>
-      </c>
-      <c r="AT5">
-        <v>1.18585194567901E+18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>400</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>13333</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="8">
         <v>447778</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>9111650</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>125279007</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>1251251004</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="8">
         <v>9563419823</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="8">
         <v>58187547820</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="8">
         <v>290737409717</v>
       </c>
-      <c r="K6" s="6">
-        <v>2</v>
-      </c>
-      <c r="L6" s="6">
+      <c r="K6" s="8">
+        <v>2</v>
+      </c>
+      <c r="L6" s="8">
         <v>3</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="8">
         <v>5</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="8">
         <v>3972999029388</v>
       </c>
-      <c r="X6">
-        <v>407254</v>
-      </c>
-      <c r="Y6">
-        <v>21591496</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>230282157</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>1251251004</v>
-      </c>
-      <c r="AB6" s="5">
-        <v>4677232746</v>
-      </c>
-      <c r="AC6" s="5">
-        <v>13777258407</v>
-      </c>
-      <c r="AD6" s="5">
-        <v>34403401347</v>
-      </c>
-      <c r="AE6">
-        <v>76095935946</v>
-      </c>
-      <c r="AF6">
-        <v>153386909107</v>
-      </c>
-      <c r="AG6">
-        <v>287302124354</v>
-      </c>
-      <c r="AH6">
-        <v>507061538596</v>
-      </c>
-      <c r="AI6">
-        <v>851978071757</v>
-      </c>
-      <c r="AJ6">
-        <v>1373554828954</v>
-      </c>
-      <c r="AK6">
-        <v>2137780735339</v>
-      </c>
-      <c r="AL6">
-        <v>3227624583857</v>
-      </c>
-      <c r="AM6">
-        <v>18009528118246</v>
-      </c>
-      <c r="AN6">
-        <v>203717871698607</v>
-      </c>
-      <c r="AO6">
-        <v>1140639187958100</v>
-      </c>
-      <c r="AP6">
-        <v>4342096628285490</v>
-      </c>
-      <c r="AQ6">
-        <v>2.7673214339696E+17</v>
-      </c>
-      <c r="AR6">
-        <v>1.76737460360657E+19</v>
-      </c>
-      <c r="AS6">
-        <v>2.01174232157437E+20</v>
-      </c>
-      <c r="AT6">
-        <v>1.12993337569593E+21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>500</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>20833</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>873264</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>22136264</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>378149106</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>4677232746</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="8">
         <v>44100541271</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="8">
         <v>329567334191</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="8">
         <v>2012762670309</v>
       </c>
-      <c r="K7" s="6">
-        <v>2</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="K7" s="8">
+        <v>2</v>
+      </c>
+      <c r="L7" s="8">
         <v>3</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="8">
         <v>5</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="8">
         <v>230793554364681</v>
       </c>
-      <c r="X7">
-        <v>930912</v>
-      </c>
-      <c r="Y7">
-        <v>87914929</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>1348858067</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>9563419823</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>44100541271</v>
-      </c>
-      <c r="AC7" s="5">
-        <v>154504465228</v>
-      </c>
-      <c r="AD7" s="5">
-        <v>447249407247</v>
-      </c>
-      <c r="AE7">
-        <v>1125143036082</v>
-      </c>
-      <c r="AF7">
-        <v>2541858922420</v>
-      </c>
-      <c r="AG7">
-        <v>5274078114658</v>
-      </c>
-      <c r="AH7">
-        <v>10213720000299</v>
-      </c>
-      <c r="AI7">
-        <v>18682742611831</v>
-      </c>
-      <c r="AJ7">
-        <v>32572992535850</v>
-      </c>
-      <c r="AK7">
-        <v>54513584583967</v>
-      </c>
-      <c r="AL7">
-        <v>88068291384398</v>
-      </c>
-      <c r="AM7">
-        <v>652203260080370</v>
-      </c>
-      <c r="AN7">
-        <v>1.10153245218577E+16</v>
-      </c>
-      <c r="AO7">
-        <v>8.2044581957463008E+16</v>
-      </c>
-      <c r="AP7">
-        <v>3.8985835339933798E+17</v>
-      </c>
-      <c r="AQ7">
-        <v>4.9554823670218498E+19</v>
-      </c>
-      <c r="AR7">
-        <v>6.3208891385988E+21</v>
-      </c>
-      <c r="AS7">
-        <v>1.07872498035519E+23</v>
-      </c>
-      <c r="AT7">
-        <v>8.0766023856325005E+23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>600</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>30000</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>1507500</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>45751225</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>934066670</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>13777258407</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>154504465228</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>1369195210284</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <v>9883035101087</v>
       </c>
-      <c r="K8" s="5">
-        <v>2</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="K8" s="3">
+        <v>2</v>
+      </c>
+      <c r="L8" s="3">
         <v>3</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>5</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>9253082936723600</v>
       </c>
-      <c r="X8">
-        <v>1786528</v>
-      </c>
-      <c r="Y8">
-        <v>290766028</v>
-      </c>
-      <c r="Z8" s="6">
-        <v>6333941094</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>58187547820</v>
-      </c>
-      <c r="AB8" s="6">
-        <v>329567334191</v>
-      </c>
-      <c r="AC8" s="5">
-        <v>1369195210284</v>
-      </c>
-      <c r="AD8" s="5">
-        <v>4584593125931</v>
-      </c>
-      <c r="AE8">
-        <v>13096052352454</v>
-      </c>
-      <c r="AF8">
-        <v>33116063658307</v>
-      </c>
-      <c r="AG8">
-        <v>76037051194142</v>
-      </c>
-      <c r="AH8">
-        <v>161437810222893</v>
-      </c>
-      <c r="AI8">
-        <v>321246606137759</v>
-      </c>
-      <c r="AJ8">
-        <v>605326449545154</v>
-      </c>
-      <c r="AK8">
-        <v>1088775619507180</v>
-      </c>
-      <c r="AL8">
-        <v>1881264064337910</v>
-      </c>
-      <c r="AM8">
-        <v>1.84611298173173E+16</v>
-      </c>
-      <c r="AN8">
-        <v>4.6478725099977901E+17</v>
-      </c>
-      <c r="AO8">
-        <v>4.60134347264691E+18</v>
-      </c>
-      <c r="AP8">
-        <v>2.7279292827788702E+19</v>
-      </c>
-      <c r="AQ8">
-        <v>6.9087707290873899E+21</v>
-      </c>
-      <c r="AR8">
-        <v>1.7591387165348501E+24</v>
-      </c>
-      <c r="AS8">
-        <v>4.50038086335053E+25</v>
-      </c>
-      <c r="AT8">
-        <v>4.4912640746291998E+26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>700</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>40833</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>2392153</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>84560700</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>2008283517</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>34403401347</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>447249407247</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>4584593125931</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>38185308620564</v>
       </c>
-      <c r="K9" s="5">
-        <v>2</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="K9" s="3">
+        <v>2</v>
+      </c>
+      <c r="L9" s="3">
         <v>3</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="3">
         <v>5</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="3">
         <v>2.7936332848370202E+17</v>
       </c>
       <c r="O9" s="7"/>
@@ -1373,114 +917,52 @@
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
-      <c r="X9" s="7">
-        <v>2977866</v>
-      </c>
-      <c r="Y9" s="7">
-        <v>807151588</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>24613920986</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>290737409717</v>
-      </c>
-      <c r="AB9" s="6">
-        <v>2012762670309</v>
-      </c>
-      <c r="AC9" s="5">
-        <v>9883035101087</v>
-      </c>
-      <c r="AD9" s="5">
-        <v>38185308620564</v>
-      </c>
-      <c r="AE9">
-        <v>123626898222812</v>
-      </c>
-      <c r="AF9">
-        <v>349407773809712</v>
-      </c>
-      <c r="AG9">
-        <v>886745696653253</v>
-      </c>
-      <c r="AH9">
-        <v>2062053737498140</v>
-      </c>
-      <c r="AI9">
-        <v>4460219326165600</v>
-      </c>
-      <c r="AJ9">
-        <v>9076962366548020</v>
-      </c>
-      <c r="AK9">
-        <v>1.75360539081224E+16</v>
-      </c>
-      <c r="AL9">
-        <v>3.23902563955393E+16</v>
-      </c>
-      <c r="AM9">
-        <v>4.2040955859086298E+17</v>
-      </c>
-      <c r="AN9">
-        <v>1.5748687013194101E+19</v>
-      </c>
-      <c r="AO9">
-        <v>2.07035979156171E+20</v>
-      </c>
-      <c r="AP9">
-        <v>1.5305250421124099E+21</v>
-      </c>
-      <c r="AQ9">
-        <v>7.7144167298733097E+23</v>
-      </c>
-      <c r="AR9">
-        <v>3.9188732492306802E+26</v>
-      </c>
-      <c r="AS9">
-        <v>1.5026023070381199E+28</v>
-      </c>
-      <c r="AT9">
-        <v>1.9985876689037601E+29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>800</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>53333</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>3568889</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>144002189</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3900009866</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>76095935946</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>1125143036082</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>13096052352454</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>123626898222812</v>
       </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10">
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+      <c r="L10" s="3">
         <v>3</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="3">
         <v>5</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="3">
         <v>6.7270900517410396E+18</v>
       </c>
       <c r="O10" s="7"/>
@@ -1492,114 +974,52 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-      <c r="X10" s="6">
-        <v>2</v>
-      </c>
-      <c r="Y10" s="6">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA10" s="6">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE10">
-        <v>2</v>
-      </c>
-      <c r="AF10">
-        <v>2</v>
-      </c>
-      <c r="AG10">
-        <v>2</v>
-      </c>
-      <c r="AH10">
-        <v>2</v>
-      </c>
-      <c r="AI10">
-        <v>2</v>
-      </c>
-      <c r="AJ10">
-        <v>2</v>
-      </c>
-      <c r="AK10">
-        <v>2</v>
-      </c>
-      <c r="AL10">
-        <v>2</v>
-      </c>
-      <c r="AM10">
-        <v>2</v>
-      </c>
-      <c r="AN10">
-        <v>2</v>
-      </c>
-      <c r="AO10">
-        <v>2</v>
-      </c>
-      <c r="AP10">
-        <v>2</v>
-      </c>
-      <c r="AQ10">
-        <v>2</v>
-      </c>
-      <c r="AR10">
-        <v>2</v>
-      </c>
-      <c r="AS10">
-        <v>2</v>
-      </c>
-      <c r="AT10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>900</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>67500</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>5079375</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>230346525</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>7006303130</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>153386909107</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>2541858922420</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>33116063658307</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>349407773809712</v>
       </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3">
         <v>3</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="3">
         <v>5</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="3">
         <v>1.34508188001572E+20</v>
       </c>
       <c r="O11" s="7"/>
@@ -1611,114 +1031,52 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-      <c r="X11" s="6">
-        <v>3</v>
-      </c>
-      <c r="Y11" s="6">
-        <v>3</v>
-      </c>
-      <c r="Z11" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA11" s="6">
-        <v>3</v>
-      </c>
-      <c r="AB11" s="6">
-        <v>3</v>
-      </c>
-      <c r="AC11" s="5">
-        <v>3</v>
-      </c>
-      <c r="AD11" s="5">
-        <v>3</v>
-      </c>
-      <c r="AE11">
-        <v>3</v>
-      </c>
-      <c r="AF11">
-        <v>3</v>
-      </c>
-      <c r="AG11">
-        <v>3</v>
-      </c>
-      <c r="AH11">
-        <v>3</v>
-      </c>
-      <c r="AI11">
-        <v>3</v>
-      </c>
-      <c r="AJ11">
-        <v>3</v>
-      </c>
-      <c r="AK11">
-        <v>3</v>
-      </c>
-      <c r="AL11">
-        <v>3</v>
-      </c>
-      <c r="AM11">
-        <v>3</v>
-      </c>
-      <c r="AN11">
-        <v>3</v>
-      </c>
-      <c r="AO11">
-        <v>3</v>
-      </c>
-      <c r="AP11">
-        <v>3</v>
-      </c>
-      <c r="AQ11">
-        <v>3</v>
-      </c>
-      <c r="AR11">
-        <v>3</v>
-      </c>
-      <c r="AS11">
-        <v>3</v>
-      </c>
-      <c r="AT11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>83333</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>6965278</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>350697875</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>11835956777</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>287302124354</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>5274078114658</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>76037051194142</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>886745696653253</v>
       </c>
-      <c r="K12">
-        <v>2</v>
-      </c>
-      <c r="L12">
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3">
         <v>3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="3">
         <v>5</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="3">
         <v>2.3001650325743201E+21</v>
       </c>
       <c r="O12" s="7"/>
@@ -1730,114 +1088,52 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="6">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="6">
-        <v>5</v>
-      </c>
-      <c r="Z12" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA12" s="6">
-        <v>5</v>
-      </c>
-      <c r="AB12" s="6">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="5">
-        <v>5</v>
-      </c>
-      <c r="AD12" s="5">
-        <v>5</v>
-      </c>
-      <c r="AE12">
-        <v>5</v>
-      </c>
-      <c r="AF12">
-        <v>5</v>
-      </c>
-      <c r="AG12">
-        <v>5</v>
-      </c>
-      <c r="AH12">
-        <v>5</v>
-      </c>
-      <c r="AI12">
-        <v>5</v>
-      </c>
-      <c r="AJ12">
-        <v>5</v>
-      </c>
-      <c r="AK12">
-        <v>5</v>
-      </c>
-      <c r="AL12">
-        <v>5</v>
-      </c>
-      <c r="AM12">
-        <v>5</v>
-      </c>
-      <c r="AN12">
-        <v>5</v>
-      </c>
-      <c r="AO12">
-        <v>5</v>
-      </c>
-      <c r="AP12">
-        <v>5</v>
-      </c>
-      <c r="AQ12">
-        <v>5</v>
-      </c>
-      <c r="AR12">
-        <v>5</v>
-      </c>
-      <c r="AS12">
-        <v>5</v>
-      </c>
-      <c r="AT12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>1100</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>100833</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>9268264</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>512993739</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>19023389376</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>507061538596</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>10213720000299</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>161437810222893</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>2062053737498140</v>
       </c>
-      <c r="K13">
-        <v>2</v>
-      </c>
-      <c r="L13">
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
         <v>3</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="3">
         <v>5</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="3">
         <v>3.4403115367205001E+22</v>
       </c>
       <c r="O13" s="7"/>
@@ -1849,105 +1145,52 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="6">
-        <v>204226</v>
-      </c>
-      <c r="Y13" s="6">
-        <v>190569292</v>
-      </c>
-      <c r="Z13" s="6">
-        <v>40853235313</v>
-      </c>
-      <c r="AA13" s="6">
-        <v>3972999029388</v>
-      </c>
-      <c r="AB13" s="6">
-        <v>230793554364681</v>
-      </c>
-      <c r="AC13" s="5">
-        <v>9253082936723600</v>
-      </c>
-      <c r="AD13" s="5">
-        <v>2.7936332848370202E+17</v>
-      </c>
-      <c r="AE13">
-        <v>6.7270900517410396E+18</v>
-      </c>
-      <c r="AF13">
-        <v>1.34508188001572E+20</v>
-      </c>
-      <c r="AG13">
-        <v>2.3001650325743201E+21</v>
-      </c>
-      <c r="AH13">
-        <v>3.4403115367205001E+22</v>
-      </c>
-      <c r="AI13">
-        <v>4.5800478800814402E+23</v>
-      </c>
-      <c r="AJ13">
-        <v>5.5036377624997203E+24</v>
-      </c>
-      <c r="AK13">
-        <v>6.0378285202834401E+25</v>
-      </c>
-      <c r="AL13">
-        <v>6.1045074711796603E+26</v>
-      </c>
-      <c r="AM13">
-        <v>2.4061467864032602E+31</v>
-      </c>
-      <c r="AN13">
-        <v>1.32946169076319E+39</v>
-      </c>
-      <c r="AO13">
-        <v>4.72081917561941E+45</v>
-      </c>
-      <c r="AP13">
-        <v>2.8708755106413501E+51</v>
-      </c>
-      <c r="AQ13">
-        <v>1.6982016882544199E+74</v>
-      </c>
-    </row>
-    <row r="14" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1200</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>120000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>12030000</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>726004950</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>29342533340</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>851978071757</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>18682742611831</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>321246606137759</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="3">
         <v>4460219326165600</v>
       </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
-      <c r="L14">
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3">
         <v>3</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="3">
         <v>5</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="3">
         <v>4.5800478800814402E+23</v>
       </c>
       <c r="O14" s="7"/>
@@ -1967,44 +1210,44 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
     </row>
-    <row r="15" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1300</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>140833</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>15292153</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>999335675</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>43720723787</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>1373554828954</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>32572992535850</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>605326449545154</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>9076962366548020</v>
       </c>
-      <c r="K15">
-        <v>2</v>
-      </c>
-      <c r="L15">
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
+      <c r="L15" s="3">
         <v>3</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="3">
         <v>5</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="3">
         <v>5.5036377624997203E+24</v>
       </c>
       <c r="O15" s="7"/>
@@ -2022,44 +1265,44 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1400</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>163333</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>19096389</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>1343423414</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>63252587636</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>2137780735339</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>54513584583967</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>1088775619507180</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>1.75360539081224E+16</v>
       </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
+      <c r="K16" s="3">
+        <v>2</v>
+      </c>
+      <c r="L16" s="3">
         <v>3</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="3">
         <v>5</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="3">
         <v>6.0378285202834401E+25</v>
       </c>
       <c r="O16" s="7"/>
@@ -2081,40 +1324,40 @@
       <c r="B17" s="1">
         <v>1500</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>187500</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>23484375</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>1769539000</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>89213932300</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>3227624583857</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>88068291384398</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>1881264064337910</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="3">
         <v>3.23902563955393E+16</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
         <v>3</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="3">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="3">
         <v>6.1045074711796603E+26</v>
       </c>
       <c r="O17" s="7"/>
@@ -2146,40 +1389,40 @@
       <c r="B18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>333333</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>55638889</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>5583347139</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>374548765406</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>18009528118246</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>652203260080370</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>1.84611298173173E+16</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="3">
         <v>4.2040955859086298E+17</v>
       </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="L18">
+      <c r="K18" s="3">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3">
         <v>3</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="3">
         <v>5</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="3">
         <v>2.4061467864032602E+31</v>
       </c>
       <c r="O18" s="7"/>
@@ -2211,40 +1454,40 @@
       <c r="B19" s="1">
         <v>3000</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>750000</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>187687500</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>28218781125</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>2833633333350</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>203717871698607</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>1.10153245218577E+16</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>4.6478725099977901E+17</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>1.5748687013194101E+19</v>
       </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-      <c r="L19">
+      <c r="K19" s="3">
+        <v>2</v>
+      </c>
+      <c r="L19" s="3">
         <v>3</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="3">
         <v>5</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="3">
         <v>1.32946169076319E+39</v>
       </c>
       <c r="O19" s="7"/>
@@ -2276,40 +1519,40 @@
       <c r="B20" s="1">
         <v>4000</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>1333333</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>444777778</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>89111166500</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>11918612345627</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>1140639187958100</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>8.2044581957463008E+16</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
         <v>4.60134347264691E+18</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="3">
         <v>2.07035979156171E+20</v>
       </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20">
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3">
         <v>3</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="3">
         <v>5</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="3">
         <v>4.72081917561941E+45</v>
       </c>
       <c r="O20" s="7"/>
@@ -2341,40 +1584,40 @@
       <c r="B21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>2083333</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>868576389</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>217448003264</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>36331925154256</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>4342096628285490</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>3.8985835339933798E+17</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>2.7279292827788702E+19</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>1.5305250421124099E+21</v>
       </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21">
+      <c r="K21" s="3">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3">
         <v>3</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="3">
         <v>5</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="3">
         <v>2.8708755106413501E+51</v>
       </c>
       <c r="O21" s="7"/>
@@ -2406,40 +1649,40 @@
       <c r="B22" s="1">
         <v>10000</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>8333333</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>6946527778</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>3475694791250</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>1160013040123320</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>2.7673214339696E+17</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>4.9554823670218498E+19</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>6.9087707290873899E+21</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="3">
         <v>7.7144167298733097E+23</v>
       </c>
-      <c r="K22">
-        <v>2</v>
-      </c>
-      <c r="L22">
+      <c r="K22" s="3">
+        <v>2</v>
+      </c>
+      <c r="L22" s="3">
         <v>3</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="3">
         <v>5</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="3">
         <v>1.6982016882544199E+74</v>
       </c>
       <c r="O22" s="7"/>
@@ -2471,39 +1714,40 @@
       <c r="B23" s="1">
         <v>20000</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>33333333</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>55563888889</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>55583334721389</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>3.7078715432098496E+16</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>1.76737460360657E+19</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>6.3208891385988E+21</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>1.7591387165348501E+24</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>3.9188732492306802E+26</v>
       </c>
-      <c r="K23">
-        <v>2</v>
-      </c>
-      <c r="L23">
+      <c r="K23" s="3">
+        <v>2</v>
+      </c>
+      <c r="L23" s="3">
         <v>3</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="3">
         <v>5</v>
       </c>
+      <c r="N23" s="4"/>
       <c r="O23" s="7"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
@@ -2533,39 +1777,40 @@
       <c r="B24" s="1">
         <v>30000</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>75000000</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>187518750000</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>281343753123750</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>2.8146097708333299E+17</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>2.01174232157437E+20</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>1.07872498035519E+23</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="3">
         <v>4.50038086335053E+25</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="3">
         <v>1.5026023070381199E+28</v>
       </c>
-      <c r="K24">
-        <v>2</v>
-      </c>
-      <c r="L24">
+      <c r="K24" s="3">
+        <v>2</v>
+      </c>
+      <c r="L24" s="3">
         <v>3</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="3">
         <v>5</v>
       </c>
+      <c r="N24" s="4"/>
       <c r="O24" s="7"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -2595,39 +1840,40 @@
       <c r="B25" s="1">
         <v>40000</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>133333333</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>444477777778</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>889111116665000</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>1.18585194567901E+18</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>1.12993337569593E+21</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>8.0766023856325005E+23</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="3">
         <v>4.4912640746291998E+26</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="3">
         <v>1.9985876689037601E+29</v>
       </c>
-      <c r="K25">
-        <v>2</v>
-      </c>
-      <c r="L25">
+      <c r="K25" s="3">
+        <v>2</v>
+      </c>
+      <c r="L25" s="3">
         <v>3</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="3">
         <v>5</v>
       </c>
+      <c r="N25" s="4"/>
       <c r="O25" s="7"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
@@ -5528,7 +4774,7 @@
   <dimension ref="B2:AF14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Counted the sets too.
</commit_message>
<xml_diff>
--- a/test/Benchmarks.xlsx
+++ b/test/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\dev\PartitionsGeneration\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDAD770-3417-4A15-A0CD-CE42BCAF0CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A10BC3C-1074-404E-AFC2-D20A8DE28ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B96E3FCC-C109-4319-B193-E4CF0B2505F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Integer Partitioning" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="14">
   <si>
     <t>TREE (n/k)</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>p(n/k)</t>
+  </si>
+  <si>
+    <t>S(n/k)</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -176,6 +186,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -184,6 +201,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -519,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B973BFE-1F92-4DF1-99F1-DD428D201207}">
   <dimension ref="B2:AP50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4757,10 +4788,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A2:A55 AT2:XFD55 B27:AS55 A56:XFD1048576 B2:N2 S14:AB14 B3:B25 Q14:Q15 Y23:AB25 Q17:Q25 R15:X25 C25:N25">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4771,10 +4802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A167EC1A-835A-434D-A2AC-FFFB0D9AA2B7}">
-  <dimension ref="B2:AF14"/>
+  <dimension ref="B2:AK66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,7 +4832,7 @@
   <sheetData>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -4843,51 +4874,6 @@
         <v>9</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="1">
-        <v>2</v>
-      </c>
-      <c r="T2" s="1">
-        <v>4</v>
-      </c>
-      <c r="U2" s="1">
-        <v>6</v>
-      </c>
-      <c r="V2" s="1">
-        <v>8</v>
-      </c>
-      <c r="W2" s="1">
-        <v>10</v>
-      </c>
-      <c r="X2" s="1">
-        <v>12</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>14</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>16</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>18</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>20</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4895,1074 +4881,2460 @@
       <c r="B3" s="1">
         <v>14</v>
       </c>
-      <c r="C3" s="3">
-        <v>44</v>
-      </c>
-      <c r="D3" s="3">
-        <v>31059</v>
-      </c>
-      <c r="E3" s="3">
-        <v>177070</v>
-      </c>
-      <c r="F3" s="3">
-        <v>77448</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3261</v>
-      </c>
-      <c r="H3" s="3">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="3">
-        <v>7</v>
-      </c>
-      <c r="N3" s="3">
-        <v>36</v>
-      </c>
-      <c r="O3" s="3">
-        <v>436</v>
-      </c>
-      <c r="P3" s="3">
-        <v>167672</v>
-      </c>
-      <c r="R3" s="1">
-        <v>14</v>
-      </c>
-      <c r="S3" s="3">
-        <v>10795</v>
-      </c>
-      <c r="T3" s="3">
-        <v>8924367</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W3" s="3">
-        <v>1878889</v>
-      </c>
-      <c r="X3" s="3">
-        <v>16997</v>
-      </c>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="3">
-        <v>1827</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>24353</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>239193</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>2</v>
+      <c r="C3" s="2">
+        <v>8191</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10391745</v>
+      </c>
+      <c r="E3" s="2">
+        <v>63436373</v>
+      </c>
+      <c r="F3" s="2">
+        <v>20912320</v>
+      </c>
+      <c r="G3" s="2">
+        <v>752752</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3367</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>91</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3367</v>
+      </c>
+      <c r="O3" s="2">
+        <v>66066</v>
+      </c>
+      <c r="P3" s="2">
+        <v>49329280</v>
       </c>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
+        <v>32767</v>
+      </c>
+      <c r="D4" s="2">
+        <v>171798901</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2734926558</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2141764053</v>
+      </c>
+      <c r="G4" s="2">
+        <v>193754990</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2757118</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6020</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
         <v>120</v>
       </c>
-      <c r="D4" s="3">
-        <v>439157</v>
-      </c>
-      <c r="E4" s="3">
-        <v>6864927</v>
-      </c>
-      <c r="F4" s="3">
-        <v>6684049</v>
-      </c>
-      <c r="G4" s="3">
-        <v>692734</v>
-      </c>
-      <c r="H4" s="3">
-        <v>18956</v>
-      </c>
-      <c r="I4" s="3">
-        <v>113</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3">
-        <v>10</v>
-      </c>
-      <c r="N4" s="3">
-        <v>91</v>
-      </c>
-      <c r="O4" s="3">
-        <v>1792</v>
-      </c>
-      <c r="P4" s="3">
-        <v>11545300</v>
-      </c>
-      <c r="R4" s="1">
-        <v>16</v>
-      </c>
-      <c r="S4" s="3">
-        <v>47816</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X4" s="3">
-        <v>10400393</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>40926</v>
-      </c>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="3">
-        <v>1097</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>65663</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>676641</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>2</v>
+      <c r="N4" s="2">
+        <v>6020</v>
+      </c>
+      <c r="O4" s="2">
+        <v>165620</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2141764053</v>
       </c>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>18</v>
       </c>
-      <c r="C5" s="3">
-        <v>772</v>
-      </c>
-      <c r="D5" s="3">
-        <v>7527032</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>111206117</v>
-      </c>
-      <c r="H5" s="3">
-        <v>4976471</v>
-      </c>
-      <c r="I5" s="3">
-        <v>59349</v>
-      </c>
-      <c r="J5" s="3">
-        <v>115</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="3">
-        <v>7</v>
-      </c>
-      <c r="N5" s="3">
-        <v>126</v>
-      </c>
-      <c r="O5" s="3">
-        <v>3134</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="1">
-        <v>18</v>
-      </c>
-      <c r="S5" s="3">
-        <v>127736</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>166203728</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>189172</v>
-      </c>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="3">
-        <v>1624</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>74668</v>
-      </c>
-      <c r="AE5" s="3">
-        <v>1793670</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>2</v>
+      <c r="C5" s="2">
+        <v>131071</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2798806985</v>
+      </c>
+      <c r="E5" s="2">
+        <v>110687251039</v>
+      </c>
+      <c r="F5" s="2">
+        <v>189036065010</v>
+      </c>
+      <c r="G5" s="2">
+        <v>37112163803</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1256328866</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8408778</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9996</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>153</v>
+      </c>
+      <c r="N5" s="2">
+        <v>9996</v>
+      </c>
+      <c r="O5" s="2">
+        <v>367200</v>
+      </c>
+      <c r="P5" s="2">
+        <v>106175395755</v>
       </c>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
-        <v>2158</v>
-      </c>
-      <c r="D6" s="3">
-        <v>111807354</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3">
-        <v>27892493</v>
-      </c>
-      <c r="J6" s="3">
-        <v>156975</v>
-      </c>
-      <c r="K6" s="3">
-        <v>194</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3">
-        <v>10</v>
-      </c>
-      <c r="N6" s="3">
-        <v>189</v>
-      </c>
-      <c r="O6" s="3">
-        <v>15162</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="1">
-        <v>20</v>
-      </c>
-      <c r="S6" s="3">
-        <v>481660</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>152254</v>
-      </c>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="3">
-        <v>2406</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>137859</v>
-      </c>
-      <c r="AE6" s="3">
-        <v>4686700</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>2</v>
+      <c r="C6" s="2">
+        <v>524287</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45232115901</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4306078895384</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15170932662679</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5917584964655</v>
+      </c>
+      <c r="H6" s="2">
+        <v>411016633391</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6302524580</v>
+      </c>
+      <c r="J6" s="2">
+        <v>22350954</v>
+      </c>
+      <c r="K6" s="2">
+        <v>15675</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>190</v>
+      </c>
+      <c r="N6" s="2">
+        <v>15675</v>
+      </c>
+      <c r="O6" s="2">
+        <v>741285</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5917584964655</v>
       </c>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
-        <v>8331</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3">
-        <v>129192183</v>
-      </c>
-      <c r="K7" s="3">
-        <v>417125</v>
-      </c>
-      <c r="L7" s="3">
-        <v>328</v>
-      </c>
-      <c r="M7" s="3">
-        <v>10</v>
-      </c>
-      <c r="N7" s="3">
-        <v>410</v>
-      </c>
-      <c r="O7" s="3">
-        <v>20911</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="1">
-        <v>22</v>
-      </c>
-      <c r="S7" s="3">
-        <v>2145556</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>289257</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>4063</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>245027</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>12414109</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>2</v>
+      <c r="C7" s="2">
+        <v>2097151</v>
+      </c>
+      <c r="D7" s="2">
+        <v>727778623825</v>
+      </c>
+      <c r="E7" s="2">
+        <v>163305339345225</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1142399079991620</v>
+      </c>
+      <c r="G7" s="2">
+        <v>835143799377954</v>
+      </c>
+      <c r="H7" s="2">
+        <v>108823356051137</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3295165281331</v>
+      </c>
+      <c r="J7" s="2">
+        <v>26046574004</v>
+      </c>
+      <c r="K7" s="2">
+        <v>53374629</v>
+      </c>
+      <c r="L7" s="2">
+        <v>23485</v>
+      </c>
+      <c r="M7" s="2">
+        <v>231</v>
+      </c>
+      <c r="N7" s="2">
+        <v>23485</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1389850</v>
+      </c>
+      <c r="P7" s="2">
+        <v>366282500870286</v>
       </c>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
-        <v>31473</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3">
-        <v>486369392</v>
-      </c>
-      <c r="L8" s="3">
-        <v>863197</v>
-      </c>
-      <c r="M8" s="3">
-        <v>13</v>
-      </c>
-      <c r="N8" s="3">
-        <v>672</v>
-      </c>
-      <c r="O8" s="3">
-        <v>62361</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="1">
-        <v>24</v>
-      </c>
-      <c r="S8" s="3">
-        <v>16090670</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="3">
-        <v>21727</v>
-      </c>
-      <c r="AD8" s="3">
-        <v>396088</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>41274616</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>2</v>
+      <c r="C8" s="2">
+        <v>8388607</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11681056634501</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6090236036084530</v>
+      </c>
+      <c r="F8" s="2">
+        <v>8.2318282158320496E+16</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.0825408178493101E+17</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2.49302045907582E+16</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1362091021641000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>20677182465555</v>
+      </c>
+      <c r="K8" s="2">
+        <v>92484925445</v>
+      </c>
+      <c r="L8" s="2">
+        <v>116972779</v>
+      </c>
+      <c r="M8" s="2">
+        <v>276</v>
+      </c>
+      <c r="N8" s="2">
+        <v>33902</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2454606</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2.49302045907582E+16</v>
       </c>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>26</v>
       </c>
-      <c r="C9" s="3">
-        <v>114816</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="3">
-        <v>35</v>
-      </c>
-      <c r="N9" s="3">
-        <v>1004</v>
-      </c>
-      <c r="O9" s="3">
-        <v>76187</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="1">
-        <v>26</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="3">
-        <v>8851</v>
-      </c>
-      <c r="AD9" s="3">
-        <v>672337</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>263048466</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>2</v>
+      <c r="C9" s="2">
+        <v>33554431</v>
+      </c>
+      <c r="D9" s="2">
+        <v>187226356946265</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.2459518697412499E+17</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5.7496222519456604E+18</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.3199555372846801E+19</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5.1495073538569503E+18</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4.77898618396288E+17</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.27258772424825E+16</v>
+      </c>
+      <c r="K9" s="2">
+        <v>107025546101760</v>
+      </c>
+      <c r="L9" s="2">
+        <v>290622864675</v>
+      </c>
+      <c r="M9" s="2">
+        <v>325</v>
+      </c>
+      <c r="N9" s="2">
+        <v>47450</v>
+      </c>
+      <c r="O9" s="2">
+        <v>4126200</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1.8505685742535501E+18</v>
       </c>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>28</v>
       </c>
-      <c r="C10" s="3">
-        <v>451968</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="3">
-        <v>29</v>
-      </c>
-      <c r="N10" s="3">
-        <v>1495</v>
-      </c>
-      <c r="O10" s="3">
-        <v>93257</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="1">
-        <v>28</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="3">
-        <v>10730</v>
-      </c>
-      <c r="AD10" s="3">
-        <v>999572</v>
-      </c>
-      <c r="AE10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="3" t="s">
-        <v>2</v>
+      <c r="C10" s="2">
+        <v>134217727</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2998587019946700</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8.2201461151886705E+18</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.9267822628136098E+20</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.53853397837477E+21</v>
+      </c>
+      <c r="H10" s="2">
+        <v>9.8539741617121303E+20</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.4878298806437501E+20</v>
+      </c>
+      <c r="J10" s="2">
+        <v>6.5396431283960402E+18</v>
+      </c>
+      <c r="K10" s="2">
+        <v>9.4432767017711808E+16</v>
+      </c>
+      <c r="L10" s="2">
+        <v>474194413703010</v>
+      </c>
+      <c r="M10" s="2">
+        <v>378</v>
+      </c>
+      <c r="N10" s="2">
+        <v>64701</v>
+      </c>
+      <c r="O10" s="2">
+        <v>6654375</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.4878298806437501E+20</v>
       </c>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>30</v>
       </c>
-      <c r="C11" s="3">
-        <v>1884762</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="3">
-        <v>19</v>
-      </c>
-      <c r="N11" s="3">
-        <v>2097</v>
-      </c>
-      <c r="O11" s="3">
-        <v>152464</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="1">
-        <v>30</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="3">
-        <v>10767</v>
-      </c>
-      <c r="AD11" s="3">
-        <v>1578376</v>
-      </c>
-      <c r="AE11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>2</v>
+      <c r="C11" s="2">
+        <v>536870911</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4.8004081105038304E+16</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.9931010274694798E+20</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.6383018684048099E+22</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.73373343599189E+23</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.77979707061075E+23</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4.2337710060168098E+22</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2.9408120982568299E+21</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6.8591811024147497E+19</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5.8153595508851098E+17</v>
+      </c>
+      <c r="M11" s="2">
+        <v>435</v>
+      </c>
+      <c r="N11" s="2">
+        <v>86275</v>
+      </c>
+      <c r="O11" s="2">
+        <v>10359090</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1.2879868072770599E+22</v>
       </c>
     </row>
     <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>35</v>
       </c>
-      <c r="C12" s="3">
-        <v>59309970</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="3">
-        <v>45</v>
-      </c>
-      <c r="N12" s="3">
-        <v>4151</v>
-      </c>
-      <c r="O12" s="3">
-        <v>445788</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R12" s="1">
-        <v>35</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="3">
-        <v>20196</v>
-      </c>
-      <c r="AD12" s="3">
-        <v>3833036</v>
-      </c>
-      <c r="AE12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF12" s="3" t="s">
-        <v>2</v>
+      <c r="C12" s="2">
+        <v>17179869183</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.9182978947632202E+19</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.3633697352056399E+24</v>
+      </c>
+      <c r="F12" s="2">
+        <v>9.3209922501882497E+26</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.1149901852685098E+28</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6.5580126734167504E+28</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4.4098913788115496E+28</v>
+      </c>
+      <c r="J12" s="2">
+        <v>8.4689238828620999E+27</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5.5323463338554997E+26</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1.37748290142564E+25</v>
+      </c>
+      <c r="M12" s="2">
+        <v>595</v>
+      </c>
+      <c r="N12" s="2">
+        <v>163625</v>
+      </c>
+      <c r="O12" s="2">
+        <v>27646080</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2.4565469823514601E+27</v>
       </c>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>40</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="3">
-        <v>56</v>
-      </c>
-      <c r="N13" s="3">
-        <v>8803</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1089082</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="1">
-        <v>40</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="3">
-        <v>34928</v>
-      </c>
-      <c r="AD13" s="3">
-        <v>9156522</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF13" s="3" t="s">
-        <v>2</v>
+      <c r="C13" s="2">
+        <v>549755813887</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.0369882873307901E+22</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.8490198597752001E+28</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3.17129794224286E+31</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.3646841252914801E+33</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.0657008257865299E+34</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3.5859872255621798E+34</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.6965203264851199E+34</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.6804473195884301E+33</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1.62188909527975E+32</v>
+      </c>
+      <c r="M13" s="2">
+        <v>780</v>
+      </c>
+      <c r="N13" s="2">
+        <v>284050</v>
+      </c>
+      <c r="O13" s="2">
+        <v>64247170</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.62188909527975E+32</v>
       </c>
     </row>
     <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>50</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="C14" s="2">
+        <v>562949953421311</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.28186553598452E+28</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.12187276309401E+36</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3.504173113261E+40</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.61547165158628E+43</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.6193309449362702E+45</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.6132809270066401E+46</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3.84008253654955E+46</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2.8189332813493401E+46</v>
+      </c>
+      <c r="L14" s="2">
+        <v>7.5979216068609797E+45</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1225</v>
+      </c>
+      <c r="N14" s="2">
+        <v>710500</v>
+      </c>
+      <c r="O14" s="2">
+        <v>259778400</v>
+      </c>
+      <c r="P14" s="2">
+        <v>7.4538021532732004E+42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1">
+        <v>18</v>
+      </c>
+      <c r="L16" s="1">
+        <v>20</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S16" s="1">
+        <v>2</v>
+      </c>
+      <c r="T16" s="1">
+        <v>4</v>
+      </c>
+      <c r="U16" s="1">
+        <v>6</v>
+      </c>
+      <c r="V16" s="1">
+        <v>8</v>
+      </c>
+      <c r="W16" s="1">
+        <v>10</v>
+      </c>
+      <c r="X16" s="1">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>16</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>18</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>20</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44</v>
+      </c>
+      <c r="D17" s="3">
+        <v>31059</v>
+      </c>
+      <c r="E17" s="3">
+        <v>177070</v>
+      </c>
+      <c r="F17" s="3">
+        <v>77448</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3261</v>
+      </c>
+      <c r="H17" s="3">
+        <v>35</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="3">
+        <v>7</v>
+      </c>
+      <c r="N17" s="3">
+        <v>36</v>
+      </c>
+      <c r="O17" s="3">
+        <v>436</v>
+      </c>
+      <c r="P17" s="3">
+        <v>167672</v>
+      </c>
+      <c r="R17" s="1">
+        <v>14</v>
+      </c>
+      <c r="S17" s="3">
+        <v>10795</v>
+      </c>
+      <c r="T17" s="3">
+        <v>8924367</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1878889</v>
+      </c>
+      <c r="X17" s="3">
+        <v>16997</v>
+      </c>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="3">
+        <v>1827</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>24353</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>239193</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3">
+        <v>120</v>
+      </c>
+      <c r="D18" s="3">
+        <v>439157</v>
+      </c>
+      <c r="E18" s="3">
+        <v>6864927</v>
+      </c>
+      <c r="F18" s="3">
+        <v>6684049</v>
+      </c>
+      <c r="G18" s="3">
+        <v>692734</v>
+      </c>
+      <c r="H18" s="3">
+        <v>18956</v>
+      </c>
+      <c r="I18" s="3">
+        <v>113</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="3">
+        <v>10</v>
+      </c>
+      <c r="N18" s="3">
+        <v>91</v>
+      </c>
+      <c r="O18" s="3">
+        <v>1792</v>
+      </c>
+      <c r="P18" s="3">
+        <v>11545300</v>
+      </c>
+      <c r="R18" s="1">
+        <v>16</v>
+      </c>
+      <c r="S18" s="3">
+        <v>47816</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X18" s="3">
+        <v>10400393</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>40926</v>
+      </c>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="3">
+        <v>1097</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>65663</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>676641</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>772</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7527032</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>111206117</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4976471</v>
+      </c>
+      <c r="I19" s="3">
+        <v>59349</v>
+      </c>
+      <c r="J19" s="3">
+        <v>115</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="3">
+        <v>7</v>
+      </c>
+      <c r="N19" s="3">
+        <v>126</v>
+      </c>
+      <c r="O19" s="3">
+        <v>3134</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R19" s="1">
+        <v>18</v>
+      </c>
+      <c r="S19" s="3">
+        <v>127736</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>166203728</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>189172</v>
+      </c>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="3">
+        <v>1624</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>74668</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>1793670</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2158</v>
+      </c>
+      <c r="D20" s="3">
+        <v>111807354</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3">
+        <v>27892493</v>
+      </c>
+      <c r="J20" s="3">
+        <v>156975</v>
+      </c>
+      <c r="K20" s="3">
+        <v>194</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="3">
+        <v>10</v>
+      </c>
+      <c r="N20" s="3">
+        <v>189</v>
+      </c>
+      <c r="O20" s="3">
+        <v>15162</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="1">
+        <v>20</v>
+      </c>
+      <c r="S20" s="3">
+        <v>481660</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>152254</v>
+      </c>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="3">
+        <v>2406</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>137859</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>4686700</v>
+      </c>
+      <c r="AF20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>22</v>
+      </c>
+      <c r="C21" s="3">
+        <v>8331</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>129192183</v>
+      </c>
+      <c r="K21" s="3">
+        <v>417125</v>
+      </c>
+      <c r="L21" s="3">
+        <v>328</v>
+      </c>
+      <c r="M21" s="3">
+        <v>10</v>
+      </c>
+      <c r="N21" s="3">
+        <v>410</v>
+      </c>
+      <c r="O21" s="3">
+        <v>20911</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="1">
+        <v>22</v>
+      </c>
+      <c r="S21" s="3">
+        <v>2145556</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>289257</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>4063</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>245027</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>12414109</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3">
+        <v>31473</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>486369392</v>
+      </c>
+      <c r="L22" s="3">
+        <v>863197</v>
+      </c>
+      <c r="M22" s="3">
+        <v>13</v>
+      </c>
+      <c r="N22" s="3">
+        <v>672</v>
+      </c>
+      <c r="O22" s="3">
+        <v>62361</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="1">
+        <v>24</v>
+      </c>
+      <c r="S22" s="3">
+        <v>16090670</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>21727</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>396088</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>41274616</v>
+      </c>
+      <c r="AF22" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3">
+        <v>114816</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="3">
+        <v>35</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1004</v>
+      </c>
+      <c r="O23" s="3">
+        <v>76187</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="1">
+        <v>26</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>8851</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>672337</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>263048466</v>
+      </c>
+      <c r="AF23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3">
+        <v>451968</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>29</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1495</v>
+      </c>
+      <c r="O24" s="3">
+        <v>93257</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R24" s="1">
+        <v>28</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>10730</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>999572</v>
+      </c>
+      <c r="AE24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF24" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>30</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1884762</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="3">
+        <v>19</v>
+      </c>
+      <c r="N25" s="3">
+        <v>2097</v>
+      </c>
+      <c r="O25" s="3">
+        <v>152464</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R25" s="1">
+        <v>30</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>10767</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>1578376</v>
+      </c>
+      <c r="AE25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>35</v>
+      </c>
+      <c r="C26" s="3">
+        <v>59309970</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>45</v>
+      </c>
+      <c r="N26" s="3">
+        <v>4151</v>
+      </c>
+      <c r="O26" s="3">
+        <v>445788</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="1">
+        <v>35</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>20196</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>3833036</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>40</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="3">
+        <v>56</v>
+      </c>
+      <c r="N27" s="3">
+        <v>8803</v>
+      </c>
+      <c r="O27" s="3">
+        <v>1089082</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R27" s="1">
+        <v>40</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>34928</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>9156522</v>
+      </c>
+      <c r="AE27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF27" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>50</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="3">
         <v>175</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N28" s="3">
         <v>31062</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O28" s="3">
         <v>5806986</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="1">
+      <c r="P28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="1">
         <v>50</v>
       </c>
-      <c r="S14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="3">
+      <c r="S28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="3">
         <v>83532</v>
       </c>
-      <c r="AD14" s="3">
+      <c r="AD28" s="3">
         <v>65501637</v>
       </c>
-      <c r="AE14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF14" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="AE28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF28" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
+    </row>
+    <row r="38" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+    </row>
+    <row r="39" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7"/>
+    </row>
+    <row r="40" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="6"/>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="6"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
+      <c r="AB40" s="6"/>
+      <c r="AC40" s="6"/>
+      <c r="AD40" s="6"/>
+      <c r="AE40" s="6"/>
+      <c r="AF40" s="6"/>
+      <c r="AG40" s="6"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
+      <c r="AJ40" s="7"/>
+      <c r="AK40" s="7"/>
+    </row>
+    <row r="41" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="6"/>
+      <c r="AE41" s="6"/>
+      <c r="AF41" s="6"/>
+      <c r="AG41" s="6"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7"/>
+    </row>
+    <row r="42" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="6"/>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+      <c r="X42" s="6"/>
+      <c r="Y42" s="6"/>
+      <c r="Z42" s="6"/>
+      <c r="AA42" s="6"/>
+      <c r="AB42" s="6"/>
+      <c r="AC42" s="6"/>
+      <c r="AD42" s="6"/>
+      <c r="AE42" s="6"/>
+      <c r="AF42" s="6"/>
+      <c r="AG42" s="6"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="7"/>
+      <c r="AJ42" s="7"/>
+      <c r="AK42" s="7"/>
+    </row>
+    <row r="43" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+      <c r="U43" s="6"/>
+      <c r="V43" s="6"/>
+      <c r="W43" s="6"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="6"/>
+      <c r="AA43" s="6"/>
+      <c r="AB43" s="6"/>
+      <c r="AC43" s="6"/>
+      <c r="AD43" s="6"/>
+      <c r="AE43" s="6"/>
+      <c r="AF43" s="6"/>
+      <c r="AG43" s="6"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7"/>
+    </row>
+    <row r="44" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+      <c r="AA44" s="6"/>
+      <c r="AB44" s="6"/>
+      <c r="AC44" s="6"/>
+      <c r="AD44" s="6"/>
+      <c r="AE44" s="6"/>
+      <c r="AF44" s="6"/>
+      <c r="AG44" s="6"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
+      <c r="AJ44" s="7"/>
+      <c r="AK44" s="7"/>
+    </row>
+    <row r="45" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+      <c r="AA45" s="6"/>
+      <c r="AB45" s="6"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="6"/>
+      <c r="AE45" s="6"/>
+      <c r="AF45" s="6"/>
+      <c r="AG45" s="6"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7"/>
+      <c r="AK45" s="7"/>
+    </row>
+    <row r="46" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+      <c r="U46" s="6"/>
+      <c r="V46" s="6"/>
+      <c r="W46" s="6"/>
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6"/>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6"/>
+      <c r="AE46" s="6"/>
+      <c r="AF46" s="6"/>
+      <c r="AG46" s="6"/>
+      <c r="AH46" s="7"/>
+      <c r="AI46" s="7"/>
+      <c r="AJ46" s="7"/>
+      <c r="AK46" s="7"/>
+    </row>
+    <row r="47" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
+      <c r="U47" s="6"/>
+      <c r="V47" s="6"/>
+      <c r="W47" s="6"/>
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6"/>
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6"/>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6"/>
+      <c r="AE47" s="6"/>
+      <c r="AF47" s="6"/>
+      <c r="AG47" s="6"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7"/>
+      <c r="AK47" s="7"/>
+    </row>
+    <row r="48" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="6"/>
+      <c r="T48" s="6"/>
+      <c r="U48" s="6"/>
+      <c r="V48" s="6"/>
+      <c r="W48" s="6"/>
+      <c r="X48" s="6"/>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6"/>
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6"/>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6"/>
+      <c r="AE48" s="6"/>
+      <c r="AF48" s="6"/>
+      <c r="AG48" s="6"/>
+      <c r="AH48" s="7"/>
+      <c r="AI48" s="7"/>
+      <c r="AJ48" s="7"/>
+      <c r="AK48" s="7"/>
+    </row>
+    <row r="49" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+      <c r="T49" s="6"/>
+      <c r="U49" s="6"/>
+      <c r="V49" s="6"/>
+      <c r="W49" s="6"/>
+      <c r="X49" s="6"/>
+      <c r="Y49" s="6"/>
+      <c r="Z49" s="6"/>
+      <c r="AA49" s="6"/>
+      <c r="AB49" s="6"/>
+      <c r="AC49" s="6"/>
+      <c r="AD49" s="6"/>
+      <c r="AE49" s="6"/>
+      <c r="AF49" s="6"/>
+      <c r="AG49" s="6"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+      <c r="AK49" s="7"/>
+    </row>
+    <row r="50" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="6"/>
+      <c r="T50" s="6"/>
+      <c r="U50" s="6"/>
+      <c r="V50" s="6"/>
+      <c r="W50" s="6"/>
+      <c r="X50" s="6"/>
+      <c r="Y50" s="6"/>
+      <c r="Z50" s="6"/>
+      <c r="AA50" s="6"/>
+      <c r="AB50" s="6"/>
+      <c r="AC50" s="6"/>
+      <c r="AD50" s="6"/>
+      <c r="AE50" s="6"/>
+      <c r="AF50" s="6"/>
+      <c r="AG50" s="6"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7"/>
+      <c r="AK50" s="7"/>
+    </row>
+    <row r="51" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
+      <c r="U51" s="6"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="6"/>
+      <c r="AG51" s="6"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7"/>
+    </row>
+    <row r="52" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="6"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="6"/>
+      <c r="AF52" s="6"/>
+      <c r="AG52" s="6"/>
+      <c r="AH52" s="7"/>
+      <c r="AI52" s="7"/>
+      <c r="AJ52" s="7"/>
+      <c r="AK52" s="7"/>
+    </row>
+    <row r="53" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="6"/>
+      <c r="AB53" s="6"/>
+      <c r="AC53" s="6"/>
+      <c r="AD53" s="6"/>
+      <c r="AE53" s="6"/>
+      <c r="AF53" s="6"/>
+      <c r="AG53" s="6"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7"/>
+    </row>
+    <row r="54" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="6"/>
+      <c r="AA54" s="6"/>
+      <c r="AB54" s="6"/>
+      <c r="AC54" s="6"/>
+      <c r="AD54" s="6"/>
+      <c r="AE54" s="6"/>
+      <c r="AF54" s="6"/>
+      <c r="AG54" s="6"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="7"/>
+      <c r="AJ54" s="7"/>
+      <c r="AK54" s="7"/>
+    </row>
+    <row r="55" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="Y55" s="6"/>
+      <c r="Z55" s="6"/>
+      <c r="AA55" s="6"/>
+      <c r="AB55" s="6"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55" s="6"/>
+      <c r="AE55" s="6"/>
+      <c r="AF55" s="6"/>
+      <c r="AG55" s="6"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+      <c r="AK55" s="7"/>
+    </row>
+    <row r="56" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+      <c r="U56" s="6"/>
+      <c r="V56" s="6"/>
+      <c r="W56" s="6"/>
+      <c r="X56" s="6"/>
+      <c r="Y56" s="6"/>
+      <c r="Z56" s="6"/>
+      <c r="AA56" s="6"/>
+      <c r="AB56" s="6"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="6"/>
+      <c r="AE56" s="6"/>
+      <c r="AF56" s="6"/>
+      <c r="AG56" s="6"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="7"/>
+      <c r="AJ56" s="7"/>
+      <c r="AK56" s="7"/>
+    </row>
+    <row r="57" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+      <c r="X57" s="6"/>
+      <c r="Y57" s="6"/>
+      <c r="Z57" s="6"/>
+      <c r="AA57" s="6"/>
+      <c r="AB57" s="6"/>
+      <c r="AC57" s="6"/>
+      <c r="AD57" s="6"/>
+      <c r="AE57" s="6"/>
+      <c r="AF57" s="6"/>
+      <c r="AG57" s="6"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+      <c r="AK57" s="7"/>
+    </row>
+    <row r="58" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
+      <c r="AA58" s="6"/>
+      <c r="AB58" s="6"/>
+      <c r="AC58" s="6"/>
+      <c r="AD58" s="6"/>
+      <c r="AE58" s="6"/>
+      <c r="AF58" s="6"/>
+      <c r="AG58" s="6"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="7"/>
+      <c r="AJ58" s="7"/>
+      <c r="AK58" s="7"/>
+    </row>
+    <row r="59" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="6"/>
+      <c r="AE59" s="6"/>
+      <c r="AF59" s="6"/>
+      <c r="AG59" s="6"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7"/>
+      <c r="AK59" s="7"/>
+    </row>
+    <row r="60" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="6"/>
+      <c r="AB60" s="6"/>
+      <c r="AC60" s="6"/>
+      <c r="AD60" s="6"/>
+      <c r="AE60" s="6"/>
+      <c r="AF60" s="6"/>
+      <c r="AG60" s="6"/>
+      <c r="AH60" s="7"/>
+      <c r="AI60" s="7"/>
+      <c r="AJ60" s="7"/>
+      <c r="AK60" s="7"/>
+    </row>
+    <row r="61" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="7"/>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7"/>
+      <c r="AC61" s="7"/>
+      <c r="AD61" s="7"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7"/>
+      <c r="AK61" s="7"/>
+    </row>
+    <row r="62" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="7"/>
+      <c r="AB62" s="7"/>
+      <c r="AC62" s="7"/>
+      <c r="AD62" s="7"/>
+      <c r="AE62" s="7"/>
+      <c r="AF62" s="7"/>
+      <c r="AG62" s="7"/>
+      <c r="AH62" s="7"/>
+      <c r="AI62" s="7"/>
+      <c r="AJ62" s="7"/>
+      <c r="AK62" s="7"/>
+    </row>
+    <row r="63" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7"/>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7"/>
+      <c r="AC63" s="7"/>
+      <c r="AD63" s="7"/>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7"/>
+      <c r="AK63" s="7"/>
+    </row>
+    <row r="64" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="7"/>
+      <c r="AB64" s="7"/>
+      <c r="AC64" s="7"/>
+      <c r="AD64" s="7"/>
+      <c r="AE64" s="7"/>
+      <c r="AF64" s="7"/>
+      <c r="AG64" s="7"/>
+      <c r="AH64" s="7"/>
+      <c r="AI64" s="7"/>
+      <c r="AJ64" s="7"/>
+      <c r="AK64" s="7"/>
+    </row>
+    <row r="65" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
+      <c r="AC65" s="7"/>
+      <c r="AD65" s="7"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="7"/>
+    </row>
+    <row r="66" spans="16:37" x14ac:dyDescent="0.25">
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7"/>
+      <c r="T66" s="7"/>
+      <c r="U66" s="7"/>
+      <c r="V66" s="7"/>
+      <c r="W66" s="7"/>
+      <c r="X66" s="7"/>
+      <c r="Y66" s="7"/>
+      <c r="Z66" s="7"/>
+      <c r="AA66" s="7"/>
+      <c r="AB66" s="7"/>
+      <c r="AC66" s="7"/>
+      <c r="AD66" s="7"/>
+      <c r="AE66" s="7"/>
+      <c r="AF66" s="7"/>
+      <c r="AG66" s="7"/>
+      <c r="AH66" s="7"/>
+      <c r="AI66" s="7"/>
+      <c r="AJ66" s="7"/>
+      <c r="AK66" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:M14 R2:AC14 AO2:XFD14 A15:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:B16 O15:XFD16 A17:XFD1048576 A2:P14">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"CRASH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A2:AF14 AO2:XFD14 A15:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1 AO2:XFD14 A15:B16 O15:XFD16 A17:XFD1048576 A2:P14">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"TIME"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:N16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"CRASH"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:N16">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"TIME"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>